<commit_message>
LE0701: Escaleta y recurso removido
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/Escaleta_LE_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/Escaleta_LE_07_01_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Lenguaje\fuentes\contenidos\grado07\guion01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25603" windowHeight="14483"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -13,13 +18,13 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -1535,19 +1540,19 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1841,7 +1846,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1851,126 +1856,126 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="R29" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3:U56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.46484375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.46484375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.83203125" style="48" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.796875" style="48" customWidth="1"/>
+    <col min="6" max="6" width="10.796875" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="62.6640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.46484375" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="47.33203125" style="46" customWidth="1"/>
-    <col min="11" max="11" width="20.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="20.46484375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.46484375" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1328125" style="7" customWidth="1"/>
     <col min="14" max="14" width="4.6640625" style="6" customWidth="1"/>
     <col min="15" max="15" width="60" style="48" customWidth="1"/>
     <col min="16" max="16" width="18.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.1640625" style="48" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.46484375" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.73046875" style="48" customWidth="1"/>
     <col min="19" max="19" width="18" style="48" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="48.83203125" style="48" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.5" style="48" bestFit="1" customWidth="1"/>
-    <col min="22" max="52" width="10.83203125" style="50"/>
-    <col min="53" max="16384" width="10.83203125" style="48"/>
+    <col min="20" max="20" width="48.796875" style="48" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.46484375" style="48" bestFit="1" customWidth="1"/>
+    <col min="22" max="52" width="10.796875" style="50"/>
+    <col min="53" max="16384" width="10.796875" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52">
-      <c r="A1" s="87" t="s">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.45">
+      <c r="A1" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="88" t="s">
+      <c r="E1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="87" t="s">
+      <c r="F1" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="87" t="s">
+      <c r="G1" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="87" t="s">
+      <c r="H1" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="87" t="s">
+      <c r="I1" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="87" t="s">
+      <c r="K1" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="87" t="s">
+      <c r="L1" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="87" t="s">
+      <c r="M1" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87" t="s">
+      <c r="N1" s="88"/>
+      <c r="O1" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="87" t="s">
+      <c r="P1" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="87" t="s">
+      <c r="Q1" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="87" t="s">
+      <c r="R1" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="87" t="s">
+      <c r="S1" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="87" t="s">
+      <c r="T1" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="87" t="s">
+      <c r="U1" s="88" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:52" s="51" customFormat="1">
-      <c r="A2" s="87"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
+    <row r="2" spans="1:52" s="51" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="88"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
       <c r="M2" s="47" t="s">
         <v>86</v>
       </c>
       <c r="N2" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="87"/>
-      <c r="S2" s="87"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="87"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
       <c r="V2" s="52"/>
       <c r="W2" s="52"/>
       <c r="X2" s="52"/>
@@ -2003,7 +2008,7 @@
       <c r="AY2" s="52"/>
       <c r="AZ2" s="52"/>
     </row>
-    <row r="3" spans="1:52">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A3" s="41" t="s">
         <v>68</v>
       </c>
@@ -2049,20 +2054,20 @@
       <c r="Q3" s="13">
         <v>6</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="R3" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="S3" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T3" s="13" t="s">
+      <c r="T3" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="U3" s="13" t="s">
+      <c r="U3" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:52">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A4" s="41" t="s">
         <v>68</v>
       </c>
@@ -2108,20 +2113,20 @@
       <c r="Q4" s="13">
         <v>6</v>
       </c>
-      <c r="R4" s="13" t="s">
+      <c r="R4" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S4" s="13" t="s">
+      <c r="S4" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T4" s="13" t="s">
+      <c r="T4" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="U4" s="13" t="s">
+      <c r="U4" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:52">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A5" s="41" t="s">
         <v>68</v>
       </c>
@@ -2167,20 +2172,20 @@
       <c r="Q5" s="13">
         <v>6</v>
       </c>
-      <c r="R5" s="13" t="s">
+      <c r="R5" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="S5" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T5" s="13" t="s">
+      <c r="T5" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="U5" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="6" spans="1:52">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A6" s="41" t="s">
         <v>68</v>
       </c>
@@ -2226,20 +2231,20 @@
       <c r="Q6" s="13">
         <v>6</v>
       </c>
-      <c r="R6" s="13" t="s">
+      <c r="R6" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S6" s="13" t="s">
+      <c r="S6" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T6" s="13" t="s">
+      <c r="T6" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="U6" s="13" t="s">
+      <c r="U6" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:52">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A7" s="41" t="s">
         <v>68</v>
       </c>
@@ -2285,20 +2290,20 @@
       <c r="Q7" s="13">
         <v>6</v>
       </c>
-      <c r="R7" s="13" t="s">
+      <c r="R7" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T7" s="13" t="s">
+      <c r="T7" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="U7" s="13" t="s">
+      <c r="U7" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="8" spans="1:52">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A8" s="41" t="s">
         <v>68</v>
       </c>
@@ -2344,20 +2349,20 @@
       <c r="Q8" s="13">
         <v>6</v>
       </c>
-      <c r="R8" s="13" t="s">
+      <c r="R8" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S8" s="13" t="s">
+      <c r="S8" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T8" s="13" t="s">
+      <c r="T8" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="U8" s="13" t="s">
+      <c r="U8" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="1:52">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A9" s="41" t="s">
         <v>68</v>
       </c>
@@ -2401,20 +2406,20 @@
       <c r="Q9" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="R9" s="20" t="s">
+      <c r="R9" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="S9" s="20" t="s">
+      <c r="S9" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="T9" s="20" t="s">
+      <c r="T9" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="U9" s="20" t="s">
+      <c r="U9" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:52">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A10" s="41" t="s">
         <v>68</v>
       </c>
@@ -2460,20 +2465,20 @@
       <c r="Q10" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="R10" s="20" t="s">
+      <c r="R10" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="S10" s="20" t="s">
+      <c r="S10" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="T10" s="20" t="s">
+      <c r="T10" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="U10" s="20" t="s">
+      <c r="U10" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:52">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A11" s="41" t="s">
         <v>68</v>
       </c>
@@ -2519,20 +2524,20 @@
       <c r="Q11" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="R11" s="20" t="s">
+      <c r="R11" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="S11" s="20" t="s">
+      <c r="S11" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="T11" s="20" t="s">
+      <c r="T11" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="U11" s="20" t="s">
+      <c r="U11" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:52">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A12" s="41" t="s">
         <v>68</v>
       </c>
@@ -2580,20 +2585,20 @@
       <c r="Q12" s="20">
         <v>6</v>
       </c>
-      <c r="R12" s="20" t="s">
+      <c r="R12" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="S12" s="20" t="s">
+      <c r="S12" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="T12" s="20" t="s">
+      <c r="T12" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="U12" s="20" t="s">
+      <c r="U12" s="17" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:52">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A13" s="41" t="s">
         <v>68</v>
       </c>
@@ -2639,20 +2644,20 @@
       <c r="Q13" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="R13" s="20" t="s">
+      <c r="R13" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="S13" s="20" t="s">
+      <c r="S13" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="T13" s="20" t="s">
+      <c r="T13" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="U13" s="20" t="s">
+      <c r="U13" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:52">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A14" s="41" t="s">
         <v>68</v>
       </c>
@@ -2700,20 +2705,20 @@
       <c r="Q14" s="20">
         <v>6</v>
       </c>
-      <c r="R14" s="20" t="s">
+      <c r="R14" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="S14" s="20" t="s">
+      <c r="S14" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="T14" s="20" t="s">
+      <c r="T14" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="U14" s="20" t="s">
+      <c r="U14" s="17" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="15" spans="1:52">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A15" s="41" t="s">
         <v>68</v>
       </c>
@@ -2759,20 +2764,20 @@
       <c r="Q15" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="R15" s="20" t="s">
+      <c r="R15" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="S15" s="20" t="s">
+      <c r="S15" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="T15" s="20" t="s">
+      <c r="T15" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="U15" s="20" t="s">
+      <c r="U15" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:52">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A16" s="41" t="s">
         <v>68</v>
       </c>
@@ -2818,20 +2823,20 @@
       <c r="Q16" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="R16" s="20" t="s">
+      <c r="R16" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="S16" s="20" t="s">
+      <c r="S16" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="T16" s="20" t="s">
+      <c r="T16" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="U16" s="20" t="s">
+      <c r="U16" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A17" s="41" t="s">
         <v>68</v>
       </c>
@@ -2877,20 +2882,20 @@
       <c r="Q17" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="R17" s="20" t="s">
+      <c r="R17" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="S17" s="20" t="s">
+      <c r="S17" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="T17" s="20" t="s">
+      <c r="T17" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="U17" s="20" t="s">
+      <c r="U17" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A18" s="41" t="s">
         <v>68</v>
       </c>
@@ -2936,20 +2941,20 @@
       <c r="Q18" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="R18" s="20" t="s">
+      <c r="R18" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="S18" s="20" t="s">
+      <c r="S18" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="T18" s="20" t="s">
+      <c r="T18" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="U18" s="20" t="s">
+      <c r="U18" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A19" s="41" t="s">
         <v>68</v>
       </c>
@@ -2997,20 +3002,20 @@
       <c r="Q19" s="20">
         <v>6</v>
       </c>
-      <c r="R19" s="20" t="s">
+      <c r="R19" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="S19" s="20" t="s">
+      <c r="S19" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="T19" s="20" t="s">
+      <c r="T19" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="U19" s="20" t="s">
+      <c r="U19" s="17" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A20" s="41" t="s">
         <v>68</v>
       </c>
@@ -3056,20 +3061,20 @@
       <c r="Q20" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="R20" s="20" t="s">
+      <c r="R20" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="S20" s="20" t="s">
+      <c r="S20" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="T20" s="20" t="s">
+      <c r="T20" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="U20" s="20" t="s">
+      <c r="U20" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A21" s="41" t="s">
         <v>68</v>
       </c>
@@ -3115,20 +3120,20 @@
       <c r="Q21" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="R21" s="20" t="s">
+      <c r="R21" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="S21" s="20" t="s">
+      <c r="S21" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="T21" s="20" t="s">
+      <c r="T21" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="U21" s="20" t="s">
+      <c r="U21" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A22" s="41" t="s">
         <v>68</v>
       </c>
@@ -3174,20 +3179,20 @@
       <c r="Q22" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="R22" s="20" t="s">
+      <c r="R22" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="S22" s="20" t="s">
+      <c r="S22" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="T22" s="20" t="s">
+      <c r="T22" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="U22" s="20" t="s">
+      <c r="U22" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A23" s="41" t="s">
         <v>68</v>
       </c>
@@ -3233,20 +3238,20 @@
       <c r="Q23" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="R23" s="20" t="s">
+      <c r="R23" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="S23" s="20" t="s">
+      <c r="S23" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="T23" s="20" t="s">
+      <c r="T23" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="U23" s="20" t="s">
+      <c r="U23" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A24" s="41" t="s">
         <v>68</v>
       </c>
@@ -3294,20 +3299,20 @@
       <c r="Q24" s="20">
         <v>6</v>
       </c>
-      <c r="R24" s="20" t="s">
+      <c r="R24" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="S24" s="20" t="s">
+      <c r="S24" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="T24" s="20" t="s">
+      <c r="T24" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="U24" s="20" t="s">
+      <c r="U24" s="17" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A25" s="41" t="s">
         <v>68</v>
       </c>
@@ -3342,8 +3347,8 @@
       <c r="L25" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="M25" s="89"/>
-      <c r="N25" s="90"/>
+      <c r="M25" s="86"/>
+      <c r="N25" s="87"/>
       <c r="O25" s="63" t="s">
         <v>199</v>
       </c>
@@ -3353,20 +3358,20 @@
       <c r="Q25" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="R25" s="74" t="s">
+      <c r="R25" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="S25" s="74" t="s">
+      <c r="S25" s="67" t="s">
         <v>96</v>
       </c>
-      <c r="T25" s="74" t="s">
+      <c r="T25" s="67" t="s">
         <v>293</v>
       </c>
-      <c r="U25" s="74" t="s">
+      <c r="U25" s="67" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A26" s="67" t="s">
         <v>68</v>
       </c>
@@ -3414,20 +3419,20 @@
       <c r="Q26" s="74">
         <v>6</v>
       </c>
-      <c r="R26" s="74" t="s">
+      <c r="R26" s="67" t="s">
         <v>262</v>
       </c>
-      <c r="S26" s="74" t="s">
+      <c r="S26" s="67" t="s">
         <v>263</v>
       </c>
-      <c r="T26" s="74" t="s">
+      <c r="T26" s="67" t="s">
         <v>273</v>
       </c>
-      <c r="U26" s="74" t="s">
+      <c r="U26" s="67" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A27" s="41" t="s">
         <v>68</v>
       </c>
@@ -3473,20 +3478,20 @@
       <c r="Q27" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="R27" s="13" t="s">
+      <c r="R27" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="S27" s="13" t="s">
+      <c r="S27" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="T27" s="13" t="s">
+      <c r="T27" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="U27" s="13" t="s">
+      <c r="U27" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A28" s="41" t="s">
         <v>68</v>
       </c>
@@ -3532,20 +3537,20 @@
       <c r="Q28" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="R28" s="13" t="s">
+      <c r="R28" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="S28" s="13" t="s">
+      <c r="S28" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="T28" s="13" t="s">
+      <c r="T28" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="U28" s="13" t="s">
+      <c r="U28" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A29" s="41" t="s">
         <v>68</v>
       </c>
@@ -3591,20 +3596,20 @@
       <c r="Q29" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="R29" s="13" t="s">
+      <c r="R29" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="S29" s="13" t="s">
+      <c r="S29" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="T29" s="13" t="s">
+      <c r="T29" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="U29" s="13" t="s">
+      <c r="U29" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A30" s="41" t="s">
         <v>68</v>
       </c>
@@ -3652,20 +3657,20 @@
       <c r="Q30" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="R30" s="13" t="s">
+      <c r="R30" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="S30" s="13" t="s">
+      <c r="S30" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="T30" s="13" t="s">
+      <c r="T30" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="U30" s="13" t="s">
+      <c r="U30" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A31" s="41" t="s">
         <v>68</v>
       </c>
@@ -3713,20 +3718,20 @@
       <c r="Q31" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="R31" s="13" t="s">
+      <c r="R31" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="S31" s="13" t="s">
+      <c r="S31" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="T31" s="13" t="s">
+      <c r="T31" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="U31" s="13" t="s">
+      <c r="U31" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A32" s="41" t="s">
         <v>68</v>
       </c>
@@ -3774,20 +3779,20 @@
       <c r="Q32" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="R32" s="13" t="s">
+      <c r="R32" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="S32" s="13" t="s">
+      <c r="S32" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="T32" s="13" t="s">
+      <c r="T32" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="U32" s="13" t="s">
+      <c r="U32" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A33" s="41" t="s">
         <v>68</v>
       </c>
@@ -3835,20 +3840,20 @@
       <c r="Q33" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="R33" s="13" t="s">
+      <c r="R33" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="S33" s="13" t="s">
+      <c r="S33" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="T33" s="13" t="s">
+      <c r="T33" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="U33" s="13" t="s">
+      <c r="U33" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A34" s="41" t="s">
         <v>68</v>
       </c>
@@ -3894,20 +3899,20 @@
       <c r="Q34" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="R34" s="13" t="s">
+      <c r="R34" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="S34" s="13" t="s">
+      <c r="S34" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="T34" s="13" t="s">
+      <c r="T34" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="U34" s="13" t="s">
+      <c r="U34" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A35" s="67" t="s">
         <v>68</v>
       </c>
@@ -3955,20 +3960,20 @@
       <c r="Q35" s="74">
         <v>6</v>
       </c>
-      <c r="R35" s="74" t="s">
+      <c r="R35" s="67" t="s">
         <v>262</v>
       </c>
-      <c r="S35" s="74" t="s">
+      <c r="S35" s="67" t="s">
         <v>263</v>
       </c>
-      <c r="T35" s="74" t="s">
+      <c r="T35" s="67" t="s">
         <v>284</v>
       </c>
-      <c r="U35" s="74" t="s">
+      <c r="U35" s="67" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="36" spans="1:21">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A36" s="41" t="s">
         <v>68</v>
       </c>
@@ -4016,20 +4021,20 @@
       <c r="Q36" s="13">
         <v>6</v>
       </c>
-      <c r="R36" s="13" t="s">
+      <c r="R36" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S36" s="13" t="s">
+      <c r="S36" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T36" s="13" t="s">
+      <c r="T36" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="U36" s="13" t="s">
+      <c r="U36" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="1:21">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A37" s="41" t="s">
         <v>68</v>
       </c>
@@ -4077,20 +4082,20 @@
       <c r="Q37" s="13">
         <v>6</v>
       </c>
-      <c r="R37" s="13" t="s">
+      <c r="R37" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S37" s="13" t="s">
+      <c r="S37" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T37" s="13" t="s">
+      <c r="T37" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="U37" s="13" t="s">
+      <c r="U37" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="38" spans="1:21">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A38" s="41" t="s">
         <v>68</v>
       </c>
@@ -4136,20 +4141,20 @@
       <c r="Q38" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="R38" s="13" t="s">
+      <c r="R38" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="S38" s="13" t="s">
+      <c r="S38" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="T38" s="13" t="s">
+      <c r="T38" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="U38" s="13" t="s">
+      <c r="U38" s="14" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:21">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A39" s="41" t="s">
         <v>68</v>
       </c>
@@ -4195,20 +4200,20 @@
       <c r="Q39" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="R39" s="13" t="s">
+      <c r="R39" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="S39" s="13" t="s">
+      <c r="S39" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="T39" s="16" t="s">
+      <c r="T39" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="U39" s="16" t="s">
+      <c r="U39" s="15" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:21">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A40" s="41" t="s">
         <v>68</v>
       </c>
@@ -4254,20 +4259,20 @@
       <c r="Q40" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="R40" s="13" t="s">
+      <c r="R40" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="S40" s="13" t="s">
+      <c r="S40" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="T40" s="16" t="s">
+      <c r="T40" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="U40" s="16" t="s">
+      <c r="U40" s="15" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:21">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A41" s="41" t="s">
         <v>68</v>
       </c>
@@ -4315,20 +4320,20 @@
       <c r="Q41" s="13">
         <v>6</v>
       </c>
-      <c r="R41" s="13" t="s">
+      <c r="R41" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S41" s="13" t="s">
+      <c r="S41" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T41" s="13" t="s">
+      <c r="T41" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="U41" s="13" t="s">
+      <c r="U41" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="42" spans="1:21">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A42" s="41" t="s">
         <v>68</v>
       </c>
@@ -4376,20 +4381,20 @@
       <c r="Q42" s="13">
         <v>6</v>
       </c>
-      <c r="R42" s="13" t="s">
+      <c r="R42" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="S42" s="13" t="s">
+      <c r="S42" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="T42" s="13" t="s">
+      <c r="T42" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="U42" s="13" t="s">
+      <c r="U42" s="14" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="43" spans="1:21">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A43" s="41" t="s">
         <v>68</v>
       </c>
@@ -4437,20 +4442,20 @@
       <c r="Q43" s="13">
         <v>6</v>
       </c>
-      <c r="R43" s="13" t="s">
+      <c r="R43" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S43" s="13" t="s">
+      <c r="S43" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T43" s="13" t="s">
+      <c r="T43" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="U43" s="13" t="s">
+      <c r="U43" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="44" spans="1:21">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A44" s="41" t="s">
         <v>68</v>
       </c>
@@ -4498,20 +4503,20 @@
       <c r="Q44" s="13">
         <v>6</v>
       </c>
-      <c r="R44" s="13" t="s">
+      <c r="R44" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S44" s="13" t="s">
+      <c r="S44" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T44" s="13" t="s">
+      <c r="T44" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="U44" s="13" t="s">
+      <c r="U44" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="45" spans="1:21">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A45" s="41" t="s">
         <v>68</v>
       </c>
@@ -4559,20 +4564,20 @@
       <c r="Q45" s="13">
         <v>6</v>
       </c>
-      <c r="R45" s="13" t="s">
+      <c r="R45" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S45" s="13" t="s">
+      <c r="S45" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T45" s="13" t="s">
+      <c r="T45" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="U45" s="13" t="s">
+      <c r="U45" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="46" spans="1:21">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A46" s="41" t="s">
         <v>68</v>
       </c>
@@ -4620,20 +4625,20 @@
       <c r="Q46" s="13">
         <v>6</v>
       </c>
-      <c r="R46" s="13" t="s">
+      <c r="R46" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S46" s="13" t="s">
+      <c r="S46" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T46" s="13" t="s">
+      <c r="T46" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="U46" s="13" t="s">
+      <c r="U46" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="47" spans="1:21">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A47" s="41" t="s">
         <v>68</v>
       </c>
@@ -4681,20 +4686,20 @@
       <c r="Q47" s="13">
         <v>6</v>
       </c>
-      <c r="R47" s="13" t="s">
+      <c r="R47" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="S47" s="13" t="s">
+      <c r="S47" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="T47" s="13" t="s">
+      <c r="T47" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="U47" s="13" t="s">
+      <c r="U47" s="14" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="48" spans="1:21">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A48" s="67" t="s">
         <v>68</v>
       </c>
@@ -4742,20 +4747,20 @@
       <c r="Q48" s="74">
         <v>6</v>
       </c>
-      <c r="R48" s="74" t="s">
+      <c r="R48" s="67" t="s">
         <v>262</v>
       </c>
-      <c r="S48" s="74" t="s">
+      <c r="S48" s="67" t="s">
         <v>263</v>
       </c>
-      <c r="T48" s="74" t="s">
+      <c r="T48" s="67" t="s">
         <v>301</v>
       </c>
-      <c r="U48" s="74" t="s">
+      <c r="U48" s="67" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="49" spans="1:52" s="63" customFormat="1">
+    <row r="49" spans="1:52" s="63" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A49" s="41" t="s">
         <v>68</v>
       </c>
@@ -4799,16 +4804,16 @@
       <c r="Q49" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="R49" s="13" t="s">
+      <c r="R49" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="S49" s="13" t="s">
+      <c r="S49" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="T49" s="13" t="s">
+      <c r="T49" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="U49" s="13" t="s">
+      <c r="U49" s="14" t="s">
         <v>95</v>
       </c>
       <c r="V49" s="50"/>
@@ -4843,7 +4848,7 @@
       <c r="AY49" s="50"/>
       <c r="AZ49" s="50"/>
     </row>
-    <row r="50" spans="1:52" s="63" customFormat="1">
+    <row r="50" spans="1:52" s="63" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A50" s="41" t="s">
         <v>68</v>
       </c>
@@ -4887,16 +4892,16 @@
       <c r="Q50" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="R50" s="16" t="s">
+      <c r="R50" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="S50" s="13" t="s">
+      <c r="S50" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="T50" s="13" t="s">
+      <c r="T50" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="U50" s="13" t="s">
+      <c r="U50" s="14" t="s">
         <v>142</v>
       </c>
       <c r="V50" s="50"/>
@@ -4931,7 +4936,7 @@
       <c r="AY50" s="50"/>
       <c r="AZ50" s="50"/>
     </row>
-    <row r="51" spans="1:52" s="63" customFormat="1">
+    <row r="51" spans="1:52" s="63" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A51" s="41" t="s">
         <v>68</v>
       </c>
@@ -4975,16 +4980,16 @@
       <c r="Q51" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="R51" s="13" t="s">
+      <c r="R51" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="S51" s="13" t="s">
+      <c r="S51" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="T51" s="13" t="s">
+      <c r="T51" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="U51" s="13" t="s">
+      <c r="U51" s="14" t="s">
         <v>142</v>
       </c>
       <c r="V51" s="50"/>
@@ -5019,7 +5024,7 @@
       <c r="AY51" s="50"/>
       <c r="AZ51" s="50"/>
     </row>
-    <row r="52" spans="1:52" s="63" customFormat="1">
+    <row r="52" spans="1:52" s="63" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A52" s="41" t="s">
         <v>68</v>
       </c>
@@ -5065,16 +5070,16 @@
       <c r="Q52" s="13">
         <v>6</v>
       </c>
-      <c r="R52" s="13" t="s">
+      <c r="R52" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S52" s="13" t="s">
+      <c r="S52" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T52" s="13" t="s">
+      <c r="T52" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="U52" s="13" t="s">
+      <c r="U52" s="14" t="s">
         <v>265</v>
       </c>
       <c r="V52" s="50"/>
@@ -5109,7 +5114,7 @@
       <c r="AY52" s="50"/>
       <c r="AZ52" s="50"/>
     </row>
-    <row r="53" spans="1:52" s="63" customFormat="1">
+    <row r="53" spans="1:52" s="63" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A53" s="41" t="s">
         <v>68</v>
       </c>
@@ -5155,16 +5160,16 @@
       <c r="Q53" s="13">
         <v>6</v>
       </c>
-      <c r="R53" s="13" t="s">
+      <c r="R53" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="S53" s="13" t="s">
+      <c r="S53" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="T53" s="13" t="s">
+      <c r="T53" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="U53" s="13" t="s">
+      <c r="U53" s="14" t="s">
         <v>278</v>
       </c>
       <c r="V53" s="50"/>
@@ -5199,7 +5204,7 @@
       <c r="AY53" s="50"/>
       <c r="AZ53" s="50"/>
     </row>
-    <row r="54" spans="1:52" s="63" customFormat="1">
+    <row r="54" spans="1:52" s="63" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A54" s="41" t="s">
         <v>68</v>
       </c>
@@ -5235,10 +5240,10 @@
         <v>19</v>
       </c>
       <c r="Q54" s="13"/>
-      <c r="R54" s="13"/>
-      <c r="S54" s="13"/>
-      <c r="T54" s="13"/>
-      <c r="U54" s="13"/>
+      <c r="R54" s="14"/>
+      <c r="S54" s="14"/>
+      <c r="T54" s="14"/>
+      <c r="U54" s="14"/>
       <c r="V54" s="50"/>
       <c r="W54" s="50"/>
       <c r="X54" s="50"/>
@@ -5271,7 +5276,7 @@
       <c r="AY54" s="50"/>
       <c r="AZ54" s="50"/>
     </row>
-    <row r="55" spans="1:52">
+    <row r="55" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A55" s="41" t="s">
         <v>68</v>
       </c>
@@ -5315,20 +5320,20 @@
       <c r="Q55" s="13">
         <v>6</v>
       </c>
-      <c r="R55" s="13" t="s">
+      <c r="R55" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="S55" s="13" t="s">
+      <c r="S55" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="T55" s="13" t="s">
+      <c r="T55" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="U55" s="13" t="s">
+      <c r="U55" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="56" spans="1:52">
+    <row r="56" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A56" s="41" t="s">
         <v>68</v>
       </c>
@@ -5372,20 +5377,20 @@
       <c r="Q56" s="82">
         <v>6</v>
       </c>
-      <c r="R56" s="82" t="s">
+      <c r="R56" s="41" t="s">
         <v>262</v>
       </c>
-      <c r="S56" s="82" t="s">
+      <c r="S56" s="41" t="s">
         <v>263</v>
       </c>
-      <c r="T56" s="82" t="s">
+      <c r="T56" s="41" t="s">
         <v>306</v>
       </c>
-      <c r="U56" s="82" t="s">
+      <c r="U56" s="41" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="57" spans="1:52" s="84" customFormat="1">
+    <row r="57" spans="1:52" s="84" customFormat="1" x14ac:dyDescent="0.45">
       <c r="V57" s="85"/>
       <c r="W57" s="85"/>
       <c r="X57" s="85"/>
@@ -5418,7 +5423,7 @@
       <c r="AY57" s="85"/>
       <c r="AZ57" s="85"/>
     </row>
-    <row r="58" spans="1:52" s="49" customFormat="1">
+    <row r="58" spans="1:52" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A58" s="36"/>
       <c r="B58" s="36"/>
       <c r="C58" s="36"/>
@@ -5435,7 +5440,7 @@
       <c r="P58" s="38"/>
       <c r="Q58" s="38"/>
     </row>
-    <row r="59" spans="1:52" s="49" customFormat="1">
+    <row r="59" spans="1:52" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A59" s="36"/>
       <c r="B59" s="36"/>
       <c r="C59" s="36"/>
@@ -5452,7 +5457,7 @@
       <c r="P59" s="38"/>
       <c r="Q59" s="38"/>
     </row>
-    <row r="60" spans="1:52" s="49" customFormat="1">
+    <row r="60" spans="1:52" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A60" s="36"/>
       <c r="B60" s="36"/>
       <c r="C60" s="36"/>
@@ -5469,7 +5474,7 @@
       <c r="P60" s="38"/>
       <c r="Q60" s="38"/>
     </row>
-    <row r="61" spans="1:52" s="49" customFormat="1">
+    <row r="61" spans="1:52" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A61" s="36"/>
       <c r="B61" s="36"/>
       <c r="C61" s="36"/>
@@ -5486,7 +5491,7 @@
       <c r="P61" s="38"/>
       <c r="Q61" s="38"/>
     </row>
-    <row r="62" spans="1:52" s="49" customFormat="1">
+    <row r="62" spans="1:52" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A62" s="36"/>
       <c r="B62" s="36"/>
       <c r="C62" s="36"/>
@@ -5503,7 +5508,7 @@
       <c r="P62" s="38"/>
       <c r="Q62" s="38"/>
     </row>
-    <row r="63" spans="1:52" s="49" customFormat="1">
+    <row r="63" spans="1:52" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A63" s="36"/>
       <c r="B63" s="36"/>
       <c r="C63" s="36"/>
@@ -5520,7 +5525,7 @@
       <c r="P63" s="38"/>
       <c r="Q63" s="38"/>
     </row>
-    <row r="64" spans="1:52" s="49" customFormat="1">
+    <row r="64" spans="1:52" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A64" s="36"/>
       <c r="B64" s="36"/>
       <c r="C64" s="36"/>
@@ -5537,7 +5542,7 @@
       <c r="P64" s="38"/>
       <c r="Q64" s="38"/>
     </row>
-    <row r="65" spans="1:21" s="49" customFormat="1">
+    <row r="65" spans="1:21" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A65" s="36"/>
       <c r="B65" s="36"/>
       <c r="C65" s="36"/>
@@ -5554,7 +5559,7 @@
       <c r="P65" s="38"/>
       <c r="Q65" s="38"/>
     </row>
-    <row r="66" spans="1:21" s="49" customFormat="1">
+    <row r="66" spans="1:21" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A66" s="36"/>
       <c r="B66" s="36"/>
       <c r="C66" s="36"/>
@@ -5571,7 +5576,7 @@
       <c r="P66" s="38"/>
       <c r="Q66" s="38"/>
     </row>
-    <row r="67" spans="1:21" s="49" customFormat="1">
+    <row r="67" spans="1:21" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A67" s="36"/>
       <c r="B67" s="36"/>
       <c r="C67" s="36"/>
@@ -5588,7 +5593,7 @@
       <c r="P67" s="38"/>
       <c r="Q67" s="38"/>
     </row>
-    <row r="68" spans="1:21" s="49" customFormat="1">
+    <row r="68" spans="1:21" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A68" s="36"/>
       <c r="B68" s="36"/>
       <c r="C68" s="36"/>
@@ -5605,7 +5610,7 @@
       <c r="P68" s="38"/>
       <c r="Q68" s="38"/>
     </row>
-    <row r="69" spans="1:21" s="49" customFormat="1">
+    <row r="69" spans="1:21" s="49" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A69" s="36"/>
       <c r="B69" s="36"/>
       <c r="C69" s="36"/>
@@ -5622,7 +5627,7 @@
       <c r="P69" s="38"/>
       <c r="Q69" s="38"/>
     </row>
-    <row r="70" spans="1:21" s="65" customFormat="1">
+    <row r="70" spans="1:21" s="65" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A70" s="36"/>
       <c r="B70" s="36"/>
       <c r="C70" s="36"/>
@@ -5645,7 +5650,7 @@
       <c r="T70" s="49"/>
       <c r="U70" s="49"/>
     </row>
-    <row r="71" spans="1:21" s="50" customFormat="1">
+    <row r="71" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A71" s="36"/>
       <c r="B71" s="36"/>
       <c r="C71" s="36"/>
@@ -5668,7 +5673,7 @@
       <c r="T71" s="49"/>
       <c r="U71" s="49"/>
     </row>
-    <row r="72" spans="1:21" s="50" customFormat="1">
+    <row r="72" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A72" s="36"/>
       <c r="B72" s="36"/>
       <c r="C72" s="36"/>
@@ -5691,7 +5696,7 @@
       <c r="T72" s="49"/>
       <c r="U72" s="49"/>
     </row>
-    <row r="73" spans="1:21" s="50" customFormat="1">
+    <row r="73" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A73" s="36"/>
       <c r="B73" s="36"/>
       <c r="C73" s="36"/>
@@ -5714,7 +5719,7 @@
       <c r="T73" s="49"/>
       <c r="U73" s="49"/>
     </row>
-    <row r="74" spans="1:21" s="50" customFormat="1">
+    <row r="74" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A74" s="36"/>
       <c r="B74" s="36"/>
       <c r="C74" s="36"/>
@@ -5737,7 +5742,7 @@
       <c r="T74" s="49"/>
       <c r="U74" s="49"/>
     </row>
-    <row r="75" spans="1:21" s="50" customFormat="1">
+    <row r="75" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A75" s="36"/>
       <c r="B75" s="36"/>
       <c r="C75" s="36"/>
@@ -5760,7 +5765,7 @@
       <c r="T75" s="49"/>
       <c r="U75" s="49"/>
     </row>
-    <row r="76" spans="1:21" s="50" customFormat="1">
+    <row r="76" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A76" s="36"/>
       <c r="B76" s="36"/>
       <c r="C76" s="36"/>
@@ -5783,7 +5788,7 @@
       <c r="T76" s="49"/>
       <c r="U76" s="49"/>
     </row>
-    <row r="77" spans="1:21" s="50" customFormat="1">
+    <row r="77" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A77" s="36"/>
       <c r="B77" s="36"/>
       <c r="C77" s="36"/>
@@ -5806,7 +5811,7 @@
       <c r="T77" s="49"/>
       <c r="U77" s="49"/>
     </row>
-    <row r="78" spans="1:21" s="50" customFormat="1">
+    <row r="78" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A78" s="36"/>
       <c r="B78" s="36"/>
       <c r="C78" s="36"/>
@@ -5829,7 +5834,7 @@
       <c r="T78" s="49"/>
       <c r="U78" s="49"/>
     </row>
-    <row r="79" spans="1:21" s="50" customFormat="1">
+    <row r="79" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A79" s="36"/>
       <c r="B79" s="36"/>
       <c r="C79" s="36"/>
@@ -5852,7 +5857,7 @@
       <c r="T79" s="49"/>
       <c r="U79" s="49"/>
     </row>
-    <row r="80" spans="1:21" s="50" customFormat="1">
+    <row r="80" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A80" s="36"/>
       <c r="B80" s="36"/>
       <c r="C80" s="36"/>
@@ -5875,7 +5880,7 @@
       <c r="T80" s="49"/>
       <c r="U80" s="49"/>
     </row>
-    <row r="81" spans="1:21" s="50" customFormat="1">
+    <row r="81" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A81" s="36"/>
       <c r="B81" s="36"/>
       <c r="C81" s="36"/>
@@ -5898,7 +5903,7 @@
       <c r="T81" s="49"/>
       <c r="U81" s="49"/>
     </row>
-    <row r="82" spans="1:21" s="50" customFormat="1">
+    <row r="82" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A82" s="36"/>
       <c r="B82" s="36"/>
       <c r="C82" s="36"/>
@@ -5921,7 +5926,7 @@
       <c r="T82" s="49"/>
       <c r="U82" s="49"/>
     </row>
-    <row r="83" spans="1:21" s="50" customFormat="1">
+    <row r="83" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A83" s="36"/>
       <c r="B83" s="36"/>
       <c r="C83" s="36"/>
@@ -5944,7 +5949,7 @@
       <c r="T83" s="49"/>
       <c r="U83" s="49"/>
     </row>
-    <row r="84" spans="1:21" s="50" customFormat="1">
+    <row r="84" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A84" s="36"/>
       <c r="B84" s="36"/>
       <c r="C84" s="36"/>
@@ -5967,7 +5972,7 @@
       <c r="T84" s="49"/>
       <c r="U84" s="49"/>
     </row>
-    <row r="85" spans="1:21" s="50" customFormat="1">
+    <row r="85" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A85" s="36"/>
       <c r="B85" s="36"/>
       <c r="C85" s="36"/>
@@ -5990,7 +5995,7 @@
       <c r="T85" s="49"/>
       <c r="U85" s="49"/>
     </row>
-    <row r="86" spans="1:21" s="50" customFormat="1">
+    <row r="86" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A86" s="36"/>
       <c r="B86" s="36"/>
       <c r="C86" s="36"/>
@@ -6013,7 +6018,7 @@
       <c r="T86" s="49"/>
       <c r="U86" s="49"/>
     </row>
-    <row r="87" spans="1:21" s="50" customFormat="1">
+    <row r="87" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A87" s="36"/>
       <c r="B87" s="36"/>
       <c r="C87" s="36"/>
@@ -6036,7 +6041,7 @@
       <c r="T87" s="49"/>
       <c r="U87" s="49"/>
     </row>
-    <row r="88" spans="1:21" s="50" customFormat="1">
+    <row r="88" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A88" s="36"/>
       <c r="B88" s="36"/>
       <c r="C88" s="36"/>
@@ -6059,7 +6064,7 @@
       <c r="T88" s="49"/>
       <c r="U88" s="49"/>
     </row>
-    <row r="89" spans="1:21" s="50" customFormat="1">
+    <row r="89" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A89" s="36"/>
       <c r="B89" s="36"/>
       <c r="C89" s="36"/>
@@ -6082,7 +6087,7 @@
       <c r="T89" s="49"/>
       <c r="U89" s="49"/>
     </row>
-    <row r="90" spans="1:21" s="50" customFormat="1">
+    <row r="90" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A90" s="36"/>
       <c r="B90" s="36"/>
       <c r="C90" s="36"/>
@@ -6105,7 +6110,7 @@
       <c r="T90" s="49"/>
       <c r="U90" s="49"/>
     </row>
-    <row r="91" spans="1:21" s="50" customFormat="1">
+    <row r="91" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A91" s="36"/>
       <c r="B91" s="36"/>
       <c r="C91" s="36"/>
@@ -6128,7 +6133,7 @@
       <c r="T91" s="49"/>
       <c r="U91" s="49"/>
     </row>
-    <row r="92" spans="1:21" s="50" customFormat="1">
+    <row r="92" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A92" s="36"/>
       <c r="B92" s="36"/>
       <c r="C92" s="36"/>
@@ -6151,7 +6156,7 @@
       <c r="T92" s="49"/>
       <c r="U92" s="49"/>
     </row>
-    <row r="93" spans="1:21" s="50" customFormat="1">
+    <row r="93" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A93" s="36"/>
       <c r="B93" s="36"/>
       <c r="C93" s="36"/>
@@ -6174,7 +6179,7 @@
       <c r="T93" s="49"/>
       <c r="U93" s="49"/>
     </row>
-    <row r="94" spans="1:21" s="50" customFormat="1">
+    <row r="94" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A94" s="36"/>
       <c r="B94" s="36"/>
       <c r="C94" s="36"/>
@@ -6197,7 +6202,7 @@
       <c r="T94" s="49"/>
       <c r="U94" s="49"/>
     </row>
-    <row r="95" spans="1:21" s="50" customFormat="1">
+    <row r="95" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A95" s="36"/>
       <c r="B95" s="36"/>
       <c r="C95" s="36"/>
@@ -6220,7 +6225,7 @@
       <c r="T95" s="49"/>
       <c r="U95" s="49"/>
     </row>
-    <row r="96" spans="1:21" s="50" customFormat="1">
+    <row r="96" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A96" s="36"/>
       <c r="B96" s="36"/>
       <c r="C96" s="36"/>
@@ -6243,7 +6248,7 @@
       <c r="T96" s="49"/>
       <c r="U96" s="49"/>
     </row>
-    <row r="97" spans="1:21" s="50" customFormat="1">
+    <row r="97" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A97" s="36"/>
       <c r="B97" s="36"/>
       <c r="C97" s="36"/>
@@ -6266,7 +6271,7 @@
       <c r="T97" s="49"/>
       <c r="U97" s="49"/>
     </row>
-    <row r="98" spans="1:21" s="50" customFormat="1">
+    <row r="98" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A98" s="36"/>
       <c r="B98" s="36"/>
       <c r="C98" s="36"/>
@@ -6289,7 +6294,7 @@
       <c r="T98" s="49"/>
       <c r="U98" s="49"/>
     </row>
-    <row r="99" spans="1:21" s="50" customFormat="1">
+    <row r="99" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A99" s="36"/>
       <c r="B99" s="36"/>
       <c r="C99" s="36"/>
@@ -6312,7 +6317,7 @@
       <c r="T99" s="49"/>
       <c r="U99" s="49"/>
     </row>
-    <row r="100" spans="1:21" s="50" customFormat="1">
+    <row r="100" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A100" s="36"/>
       <c r="B100" s="36"/>
       <c r="C100" s="36"/>
@@ -6335,7 +6340,7 @@
       <c r="T100" s="49"/>
       <c r="U100" s="49"/>
     </row>
-    <row r="101" spans="1:21" s="50" customFormat="1">
+    <row r="101" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A101" s="36"/>
       <c r="B101" s="36"/>
       <c r="C101" s="36"/>
@@ -6358,7 +6363,7 @@
       <c r="T101" s="49"/>
       <c r="U101" s="49"/>
     </row>
-    <row r="102" spans="1:21" s="50" customFormat="1">
+    <row r="102" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A102" s="36"/>
       <c r="B102" s="36"/>
       <c r="C102" s="36"/>
@@ -6381,7 +6386,7 @@
       <c r="T102" s="49"/>
       <c r="U102" s="49"/>
     </row>
-    <row r="103" spans="1:21" s="50" customFormat="1">
+    <row r="103" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A103" s="36"/>
       <c r="B103" s="36"/>
       <c r="C103" s="36"/>
@@ -6404,7 +6409,7 @@
       <c r="T103" s="49"/>
       <c r="U103" s="49"/>
     </row>
-    <row r="104" spans="1:21" s="50" customFormat="1">
+    <row r="104" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A104" s="36"/>
       <c r="B104" s="36"/>
       <c r="C104" s="36"/>
@@ -6427,7 +6432,7 @@
       <c r="T104" s="49"/>
       <c r="U104" s="49"/>
     </row>
-    <row r="105" spans="1:21" s="50" customFormat="1">
+    <row r="105" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A105" s="36"/>
       <c r="B105" s="36"/>
       <c r="C105" s="36"/>
@@ -6450,7 +6455,7 @@
       <c r="T105" s="49"/>
       <c r="U105" s="49"/>
     </row>
-    <row r="106" spans="1:21" s="50" customFormat="1">
+    <row r="106" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A106" s="36"/>
       <c r="B106" s="36"/>
       <c r="C106" s="36"/>
@@ -6473,7 +6478,7 @@
       <c r="T106" s="49"/>
       <c r="U106" s="49"/>
     </row>
-    <row r="107" spans="1:21" s="50" customFormat="1">
+    <row r="107" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A107" s="36"/>
       <c r="B107" s="36"/>
       <c r="C107" s="36"/>
@@ -6496,7 +6501,7 @@
       <c r="T107" s="49"/>
       <c r="U107" s="49"/>
     </row>
-    <row r="108" spans="1:21" s="50" customFormat="1">
+    <row r="108" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A108" s="36"/>
       <c r="B108" s="36"/>
       <c r="C108" s="36"/>
@@ -6519,7 +6524,7 @@
       <c r="T108" s="49"/>
       <c r="U108" s="49"/>
     </row>
-    <row r="109" spans="1:21" s="50" customFormat="1">
+    <row r="109" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A109" s="36"/>
       <c r="B109" s="36"/>
       <c r="C109" s="36"/>
@@ -6542,7 +6547,7 @@
       <c r="T109" s="49"/>
       <c r="U109" s="49"/>
     </row>
-    <row r="110" spans="1:21" s="50" customFormat="1">
+    <row r="110" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A110" s="36"/>
       <c r="B110" s="36"/>
       <c r="C110" s="36"/>
@@ -6565,7 +6570,7 @@
       <c r="T110" s="49"/>
       <c r="U110" s="49"/>
     </row>
-    <row r="111" spans="1:21" s="50" customFormat="1">
+    <row r="111" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A111" s="36"/>
       <c r="B111" s="36"/>
       <c r="C111" s="36"/>
@@ -6588,7 +6593,7 @@
       <c r="T111" s="49"/>
       <c r="U111" s="49"/>
     </row>
-    <row r="112" spans="1:21" s="50" customFormat="1">
+    <row r="112" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A112" s="36"/>
       <c r="B112" s="36"/>
       <c r="C112" s="36"/>
@@ -6611,7 +6616,7 @@
       <c r="T112" s="49"/>
       <c r="U112" s="49"/>
     </row>
-    <row r="113" spans="1:21" s="50" customFormat="1">
+    <row r="113" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A113" s="36"/>
       <c r="B113" s="36"/>
       <c r="C113" s="36"/>
@@ -6634,7 +6639,7 @@
       <c r="T113" s="49"/>
       <c r="U113" s="49"/>
     </row>
-    <row r="114" spans="1:21" s="50" customFormat="1">
+    <row r="114" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A114" s="36"/>
       <c r="B114" s="36"/>
       <c r="C114" s="36"/>
@@ -6657,7 +6662,7 @@
       <c r="T114" s="49"/>
       <c r="U114" s="49"/>
     </row>
-    <row r="115" spans="1:21" s="50" customFormat="1">
+    <row r="115" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A115" s="36"/>
       <c r="B115" s="36"/>
       <c r="C115" s="36"/>
@@ -6680,7 +6685,7 @@
       <c r="T115" s="49"/>
       <c r="U115" s="49"/>
     </row>
-    <row r="116" spans="1:21" s="50" customFormat="1">
+    <row r="116" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A116" s="36"/>
       <c r="B116" s="36"/>
       <c r="C116" s="36"/>
@@ -6703,7 +6708,7 @@
       <c r="T116" s="49"/>
       <c r="U116" s="49"/>
     </row>
-    <row r="117" spans="1:21" s="50" customFormat="1">
+    <row r="117" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A117" s="36"/>
       <c r="B117" s="36"/>
       <c r="C117" s="36"/>
@@ -6726,7 +6731,7 @@
       <c r="T117" s="49"/>
       <c r="U117" s="49"/>
     </row>
-    <row r="118" spans="1:21" s="50" customFormat="1">
+    <row r="118" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A118" s="36"/>
       <c r="B118" s="36"/>
       <c r="C118" s="36"/>
@@ -6749,7 +6754,7 @@
       <c r="T118" s="49"/>
       <c r="U118" s="49"/>
     </row>
-    <row r="119" spans="1:21" s="50" customFormat="1">
+    <row r="119" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A119" s="36"/>
       <c r="B119" s="36"/>
       <c r="C119" s="36"/>
@@ -6772,7 +6777,7 @@
       <c r="T119" s="49"/>
       <c r="U119" s="49"/>
     </row>
-    <row r="120" spans="1:21" s="50" customFormat="1">
+    <row r="120" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A120" s="36"/>
       <c r="B120" s="36"/>
       <c r="C120" s="36"/>
@@ -6795,7 +6800,7 @@
       <c r="T120" s="49"/>
       <c r="U120" s="49"/>
     </row>
-    <row r="121" spans="1:21" s="50" customFormat="1">
+    <row r="121" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A121" s="36"/>
       <c r="B121" s="36"/>
       <c r="C121" s="36"/>
@@ -6818,7 +6823,7 @@
       <c r="T121" s="49"/>
       <c r="U121" s="49"/>
     </row>
-    <row r="122" spans="1:21" s="50" customFormat="1">
+    <row r="122" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A122" s="36"/>
       <c r="B122" s="36"/>
       <c r="C122" s="36"/>
@@ -6841,7 +6846,7 @@
       <c r="T122" s="49"/>
       <c r="U122" s="49"/>
     </row>
-    <row r="123" spans="1:21" s="50" customFormat="1">
+    <row r="123" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A123" s="36"/>
       <c r="B123" s="36"/>
       <c r="C123" s="36"/>
@@ -6864,7 +6869,7 @@
       <c r="T123" s="49"/>
       <c r="U123" s="49"/>
     </row>
-    <row r="124" spans="1:21" s="50" customFormat="1">
+    <row r="124" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A124" s="36"/>
       <c r="B124" s="36"/>
       <c r="C124" s="36"/>
@@ -6887,7 +6892,7 @@
       <c r="T124" s="49"/>
       <c r="U124" s="49"/>
     </row>
-    <row r="125" spans="1:21" s="50" customFormat="1">
+    <row r="125" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A125" s="36"/>
       <c r="B125" s="36"/>
       <c r="C125" s="36"/>
@@ -6910,7 +6915,7 @@
       <c r="T125" s="49"/>
       <c r="U125" s="49"/>
     </row>
-    <row r="126" spans="1:21" s="50" customFormat="1">
+    <row r="126" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A126" s="36"/>
       <c r="B126" s="36"/>
       <c r="C126" s="36"/>
@@ -6933,7 +6938,7 @@
       <c r="T126" s="49"/>
       <c r="U126" s="49"/>
     </row>
-    <row r="127" spans="1:21" s="50" customFormat="1">
+    <row r="127" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A127" s="36"/>
       <c r="B127" s="36"/>
       <c r="C127" s="36"/>
@@ -6956,7 +6961,7 @@
       <c r="T127" s="49"/>
       <c r="U127" s="49"/>
     </row>
-    <row r="128" spans="1:21" s="50" customFormat="1">
+    <row r="128" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A128" s="36"/>
       <c r="B128" s="36"/>
       <c r="C128" s="36"/>
@@ -6979,7 +6984,7 @@
       <c r="T128" s="49"/>
       <c r="U128" s="49"/>
     </row>
-    <row r="129" spans="1:21" s="50" customFormat="1">
+    <row r="129" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A129" s="36"/>
       <c r="B129" s="36"/>
       <c r="C129" s="36"/>
@@ -7002,7 +7007,7 @@
       <c r="T129" s="49"/>
       <c r="U129" s="49"/>
     </row>
-    <row r="130" spans="1:21" s="50" customFormat="1">
+    <row r="130" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A130" s="36"/>
       <c r="B130" s="36"/>
       <c r="C130" s="36"/>
@@ -7025,7 +7030,7 @@
       <c r="T130" s="49"/>
       <c r="U130" s="49"/>
     </row>
-    <row r="131" spans="1:21" s="50" customFormat="1">
+    <row r="131" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A131" s="36"/>
       <c r="B131" s="36"/>
       <c r="C131" s="36"/>
@@ -7048,7 +7053,7 @@
       <c r="T131" s="49"/>
       <c r="U131" s="49"/>
     </row>
-    <row r="132" spans="1:21" s="50" customFormat="1">
+    <row r="132" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A132" s="36"/>
       <c r="B132" s="36"/>
       <c r="C132" s="36"/>
@@ -7071,7 +7076,7 @@
       <c r="T132" s="49"/>
       <c r="U132" s="49"/>
     </row>
-    <row r="133" spans="1:21" s="50" customFormat="1">
+    <row r="133" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A133" s="36"/>
       <c r="B133" s="36"/>
       <c r="C133" s="36"/>
@@ -7094,7 +7099,7 @@
       <c r="T133" s="49"/>
       <c r="U133" s="49"/>
     </row>
-    <row r="134" spans="1:21" s="50" customFormat="1">
+    <row r="134" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A134" s="36"/>
       <c r="B134" s="36"/>
       <c r="C134" s="36"/>
@@ -7117,7 +7122,7 @@
       <c r="T134" s="49"/>
       <c r="U134" s="49"/>
     </row>
-    <row r="135" spans="1:21" s="50" customFormat="1">
+    <row r="135" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A135" s="36"/>
       <c r="B135" s="36"/>
       <c r="C135" s="36"/>
@@ -7140,7 +7145,7 @@
       <c r="T135" s="49"/>
       <c r="U135" s="49"/>
     </row>
-    <row r="136" spans="1:21" s="50" customFormat="1">
+    <row r="136" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A136" s="36"/>
       <c r="B136" s="36"/>
       <c r="C136" s="36"/>
@@ -7163,7 +7168,7 @@
       <c r="T136" s="49"/>
       <c r="U136" s="49"/>
     </row>
-    <row r="137" spans="1:21" s="50" customFormat="1">
+    <row r="137" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A137" s="36"/>
       <c r="B137" s="36"/>
       <c r="C137" s="36"/>
@@ -7186,7 +7191,7 @@
       <c r="T137" s="49"/>
       <c r="U137" s="49"/>
     </row>
-    <row r="138" spans="1:21" s="50" customFormat="1">
+    <row r="138" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A138" s="36"/>
       <c r="B138" s="36"/>
       <c r="C138" s="36"/>
@@ -7209,7 +7214,7 @@
       <c r="T138" s="49"/>
       <c r="U138" s="49"/>
     </row>
-    <row r="139" spans="1:21" s="50" customFormat="1">
+    <row r="139" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A139" s="36"/>
       <c r="B139" s="36"/>
       <c r="C139" s="36"/>
@@ -7232,7 +7237,7 @@
       <c r="T139" s="49"/>
       <c r="U139" s="49"/>
     </row>
-    <row r="140" spans="1:21" s="50" customFormat="1">
+    <row r="140" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A140" s="36"/>
       <c r="B140" s="36"/>
       <c r="C140" s="36"/>
@@ -7255,7 +7260,7 @@
       <c r="T140" s="49"/>
       <c r="U140" s="49"/>
     </row>
-    <row r="141" spans="1:21" s="50" customFormat="1">
+    <row r="141" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A141" s="36"/>
       <c r="B141" s="36"/>
       <c r="C141" s="36"/>
@@ -7278,7 +7283,7 @@
       <c r="T141" s="49"/>
       <c r="U141" s="49"/>
     </row>
-    <row r="142" spans="1:21" s="50" customFormat="1">
+    <row r="142" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A142" s="36"/>
       <c r="B142" s="36"/>
       <c r="C142" s="36"/>
@@ -7301,7 +7306,7 @@
       <c r="T142" s="49"/>
       <c r="U142" s="49"/>
     </row>
-    <row r="143" spans="1:21" s="50" customFormat="1">
+    <row r="143" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A143" s="36"/>
       <c r="B143" s="36"/>
       <c r="C143" s="36"/>
@@ -7324,7 +7329,7 @@
       <c r="T143" s="49"/>
       <c r="U143" s="49"/>
     </row>
-    <row r="144" spans="1:21" s="50" customFormat="1">
+    <row r="144" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A144" s="36"/>
       <c r="B144" s="36"/>
       <c r="C144" s="36"/>
@@ -7347,7 +7352,7 @@
       <c r="T144" s="49"/>
       <c r="U144" s="49"/>
     </row>
-    <row r="145" spans="1:21" s="50" customFormat="1">
+    <row r="145" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A145" s="36"/>
       <c r="B145" s="36"/>
       <c r="C145" s="36"/>
@@ -7370,7 +7375,7 @@
       <c r="T145" s="49"/>
       <c r="U145" s="49"/>
     </row>
-    <row r="146" spans="1:21" s="50" customFormat="1">
+    <row r="146" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A146" s="36"/>
       <c r="B146" s="36"/>
       <c r="C146" s="36"/>
@@ -7393,7 +7398,7 @@
       <c r="T146" s="49"/>
       <c r="U146" s="49"/>
     </row>
-    <row r="147" spans="1:21" s="50" customFormat="1">
+    <row r="147" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A147" s="36"/>
       <c r="B147" s="36"/>
       <c r="C147" s="36"/>
@@ -7416,7 +7421,7 @@
       <c r="T147" s="49"/>
       <c r="U147" s="49"/>
     </row>
-    <row r="148" spans="1:21" s="50" customFormat="1">
+    <row r="148" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A148" s="36"/>
       <c r="B148" s="36"/>
       <c r="C148" s="36"/>
@@ -7439,7 +7444,7 @@
       <c r="T148" s="49"/>
       <c r="U148" s="49"/>
     </row>
-    <row r="149" spans="1:21" s="50" customFormat="1">
+    <row r="149" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A149" s="36"/>
       <c r="B149" s="36"/>
       <c r="C149" s="36"/>
@@ -7462,7 +7467,7 @@
       <c r="T149" s="49"/>
       <c r="U149" s="49"/>
     </row>
-    <row r="150" spans="1:21" s="50" customFormat="1">
+    <row r="150" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A150" s="36"/>
       <c r="B150" s="36"/>
       <c r="C150" s="36"/>
@@ -7485,7 +7490,7 @@
       <c r="T150" s="49"/>
       <c r="U150" s="49"/>
     </row>
-    <row r="151" spans="1:21" s="50" customFormat="1">
+    <row r="151" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A151" s="36"/>
       <c r="B151" s="36"/>
       <c r="C151" s="36"/>
@@ -7508,7 +7513,7 @@
       <c r="T151" s="49"/>
       <c r="U151" s="49"/>
     </row>
-    <row r="152" spans="1:21" s="50" customFormat="1">
+    <row r="152" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A152" s="36"/>
       <c r="B152" s="36"/>
       <c r="C152" s="36"/>
@@ -7531,7 +7536,7 @@
       <c r="T152" s="49"/>
       <c r="U152" s="49"/>
     </row>
-    <row r="153" spans="1:21" s="50" customFormat="1">
+    <row r="153" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A153" s="36"/>
       <c r="B153" s="36"/>
       <c r="C153" s="36"/>
@@ -7554,7 +7559,7 @@
       <c r="T153" s="49"/>
       <c r="U153" s="49"/>
     </row>
-    <row r="154" spans="1:21" s="50" customFormat="1">
+    <row r="154" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A154" s="36"/>
       <c r="B154" s="36"/>
       <c r="C154" s="36"/>
@@ -7577,7 +7582,7 @@
       <c r="T154" s="49"/>
       <c r="U154" s="49"/>
     </row>
-    <row r="155" spans="1:21" s="50" customFormat="1">
+    <row r="155" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A155" s="36"/>
       <c r="B155" s="36"/>
       <c r="C155" s="36"/>
@@ -7600,7 +7605,7 @@
       <c r="T155" s="49"/>
       <c r="U155" s="49"/>
     </row>
-    <row r="156" spans="1:21" s="50" customFormat="1">
+    <row r="156" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A156" s="36"/>
       <c r="B156" s="36"/>
       <c r="C156" s="36"/>
@@ -7623,7 +7628,7 @@
       <c r="T156" s="49"/>
       <c r="U156" s="49"/>
     </row>
-    <row r="157" spans="1:21" s="50" customFormat="1">
+    <row r="157" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A157" s="36"/>
       <c r="B157" s="36"/>
       <c r="C157" s="36"/>
@@ -7646,7 +7651,7 @@
       <c r="T157" s="49"/>
       <c r="U157" s="49"/>
     </row>
-    <row r="158" spans="1:21" s="50" customFormat="1">
+    <row r="158" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A158" s="36"/>
       <c r="B158" s="36"/>
       <c r="C158" s="36"/>
@@ -7669,7 +7674,7 @@
       <c r="T158" s="49"/>
       <c r="U158" s="49"/>
     </row>
-    <row r="159" spans="1:21" s="50" customFormat="1">
+    <row r="159" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A159" s="36"/>
       <c r="B159" s="36"/>
       <c r="C159" s="36"/>
@@ -7692,7 +7697,7 @@
       <c r="T159" s="49"/>
       <c r="U159" s="49"/>
     </row>
-    <row r="160" spans="1:21" s="50" customFormat="1">
+    <row r="160" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A160" s="36"/>
       <c r="B160" s="36"/>
       <c r="C160" s="36"/>
@@ -7715,7 +7720,7 @@
       <c r="T160" s="49"/>
       <c r="U160" s="49"/>
     </row>
-    <row r="161" spans="1:21" s="50" customFormat="1">
+    <row r="161" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A161" s="36"/>
       <c r="B161" s="36"/>
       <c r="C161" s="36"/>
@@ -7738,7 +7743,7 @@
       <c r="T161" s="49"/>
       <c r="U161" s="49"/>
     </row>
-    <row r="162" spans="1:21" s="50" customFormat="1">
+    <row r="162" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A162" s="36"/>
       <c r="B162" s="36"/>
       <c r="C162" s="36"/>
@@ -7761,7 +7766,7 @@
       <c r="T162" s="49"/>
       <c r="U162" s="49"/>
     </row>
-    <row r="163" spans="1:21" s="50" customFormat="1">
+    <row r="163" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A163" s="36"/>
       <c r="B163" s="36"/>
       <c r="C163" s="36"/>
@@ -7784,7 +7789,7 @@
       <c r="T163" s="49"/>
       <c r="U163" s="49"/>
     </row>
-    <row r="164" spans="1:21" s="50" customFormat="1">
+    <row r="164" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A164" s="36"/>
       <c r="B164" s="36"/>
       <c r="C164" s="36"/>
@@ -7807,7 +7812,7 @@
       <c r="T164" s="49"/>
       <c r="U164" s="49"/>
     </row>
-    <row r="165" spans="1:21" s="50" customFormat="1">
+    <row r="165" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A165" s="36"/>
       <c r="B165" s="36"/>
       <c r="C165" s="36"/>
@@ -7830,7 +7835,7 @@
       <c r="T165" s="49"/>
       <c r="U165" s="49"/>
     </row>
-    <row r="166" spans="1:21" s="50" customFormat="1">
+    <row r="166" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A166" s="36"/>
       <c r="B166" s="36"/>
       <c r="C166" s="36"/>
@@ -7853,7 +7858,7 @@
       <c r="T166" s="49"/>
       <c r="U166" s="49"/>
     </row>
-    <row r="167" spans="1:21" s="50" customFormat="1">
+    <row r="167" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A167" s="36"/>
       <c r="B167" s="36"/>
       <c r="C167" s="36"/>
@@ -7876,7 +7881,7 @@
       <c r="T167" s="49"/>
       <c r="U167" s="49"/>
     </row>
-    <row r="168" spans="1:21" s="50" customFormat="1">
+    <row r="168" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A168" s="36"/>
       <c r="B168" s="36"/>
       <c r="C168" s="36"/>
@@ -7899,7 +7904,7 @@
       <c r="T168" s="49"/>
       <c r="U168" s="49"/>
     </row>
-    <row r="169" spans="1:21" s="50" customFormat="1">
+    <row r="169" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A169" s="36"/>
       <c r="B169" s="36"/>
       <c r="C169" s="36"/>
@@ -7922,7 +7927,7 @@
       <c r="T169" s="49"/>
       <c r="U169" s="49"/>
     </row>
-    <row r="170" spans="1:21" s="50" customFormat="1">
+    <row r="170" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A170" s="36"/>
       <c r="B170" s="36"/>
       <c r="C170" s="36"/>
@@ -7945,7 +7950,7 @@
       <c r="T170" s="49"/>
       <c r="U170" s="49"/>
     </row>
-    <row r="171" spans="1:21" s="50" customFormat="1">
+    <row r="171" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A171" s="36"/>
       <c r="B171" s="36"/>
       <c r="C171" s="36"/>
@@ -7968,7 +7973,7 @@
       <c r="T171" s="49"/>
       <c r="U171" s="49"/>
     </row>
-    <row r="172" spans="1:21" s="50" customFormat="1">
+    <row r="172" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A172" s="36"/>
       <c r="B172" s="36"/>
       <c r="C172" s="36"/>
@@ -7991,7 +7996,7 @@
       <c r="T172" s="49"/>
       <c r="U172" s="49"/>
     </row>
-    <row r="173" spans="1:21" s="50" customFormat="1">
+    <row r="173" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A173" s="36"/>
       <c r="B173" s="36"/>
       <c r="C173" s="36"/>
@@ -8014,7 +8019,7 @@
       <c r="T173" s="49"/>
       <c r="U173" s="49"/>
     </row>
-    <row r="174" spans="1:21" s="50" customFormat="1">
+    <row r="174" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A174" s="36"/>
       <c r="B174" s="36"/>
       <c r="C174" s="36"/>
@@ -8037,7 +8042,7 @@
       <c r="T174" s="49"/>
       <c r="U174" s="49"/>
     </row>
-    <row r="175" spans="1:21" s="50" customFormat="1">
+    <row r="175" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A175" s="36"/>
       <c r="B175" s="36"/>
       <c r="C175" s="36"/>
@@ -8060,7 +8065,7 @@
       <c r="T175" s="49"/>
       <c r="U175" s="49"/>
     </row>
-    <row r="176" spans="1:21" s="50" customFormat="1">
+    <row r="176" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A176" s="36"/>
       <c r="B176" s="36"/>
       <c r="C176" s="36"/>
@@ -8083,7 +8088,7 @@
       <c r="T176" s="49"/>
       <c r="U176" s="49"/>
     </row>
-    <row r="177" spans="1:21" s="50" customFormat="1">
+    <row r="177" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A177" s="36"/>
       <c r="B177" s="36"/>
       <c r="C177" s="36"/>
@@ -8106,7 +8111,7 @@
       <c r="T177" s="49"/>
       <c r="U177" s="49"/>
     </row>
-    <row r="178" spans="1:21" s="50" customFormat="1">
+    <row r="178" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A178" s="36"/>
       <c r="B178" s="36"/>
       <c r="C178" s="36"/>
@@ -8129,7 +8134,7 @@
       <c r="T178" s="49"/>
       <c r="U178" s="49"/>
     </row>
-    <row r="179" spans="1:21" s="50" customFormat="1">
+    <row r="179" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A179" s="36"/>
       <c r="B179" s="36"/>
       <c r="C179" s="36"/>
@@ -8152,7 +8157,7 @@
       <c r="T179" s="49"/>
       <c r="U179" s="49"/>
     </row>
-    <row r="180" spans="1:21" s="50" customFormat="1">
+    <row r="180" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A180" s="36"/>
       <c r="B180" s="36"/>
       <c r="C180" s="36"/>
@@ -8175,7 +8180,7 @@
       <c r="T180" s="49"/>
       <c r="U180" s="49"/>
     </row>
-    <row r="181" spans="1:21" s="50" customFormat="1">
+    <row r="181" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A181" s="36"/>
       <c r="B181" s="36"/>
       <c r="C181" s="36"/>
@@ -8198,7 +8203,7 @@
       <c r="T181" s="49"/>
       <c r="U181" s="49"/>
     </row>
-    <row r="182" spans="1:21" s="50" customFormat="1">
+    <row r="182" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A182" s="36"/>
       <c r="B182" s="36"/>
       <c r="C182" s="36"/>
@@ -8221,7 +8226,7 @@
       <c r="T182" s="49"/>
       <c r="U182" s="49"/>
     </row>
-    <row r="183" spans="1:21" s="50" customFormat="1">
+    <row r="183" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A183" s="36"/>
       <c r="B183" s="36"/>
       <c r="C183" s="36"/>
@@ -8244,7 +8249,7 @@
       <c r="T183" s="49"/>
       <c r="U183" s="49"/>
     </row>
-    <row r="184" spans="1:21" s="50" customFormat="1">
+    <row r="184" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A184" s="36"/>
       <c r="B184" s="36"/>
       <c r="C184" s="36"/>
@@ -8267,7 +8272,7 @@
       <c r="T184" s="49"/>
       <c r="U184" s="49"/>
     </row>
-    <row r="185" spans="1:21" s="50" customFormat="1">
+    <row r="185" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A185" s="36"/>
       <c r="B185" s="36"/>
       <c r="C185" s="36"/>
@@ -8290,7 +8295,7 @@
       <c r="T185" s="49"/>
       <c r="U185" s="49"/>
     </row>
-    <row r="186" spans="1:21" s="50" customFormat="1">
+    <row r="186" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A186" s="36"/>
       <c r="B186" s="36"/>
       <c r="C186" s="36"/>
@@ -8313,7 +8318,7 @@
       <c r="T186" s="49"/>
       <c r="U186" s="49"/>
     </row>
-    <row r="187" spans="1:21" s="50" customFormat="1">
+    <row r="187" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A187" s="36"/>
       <c r="B187" s="36"/>
       <c r="C187" s="36"/>
@@ -8336,7 +8341,7 @@
       <c r="T187" s="49"/>
       <c r="U187" s="49"/>
     </row>
-    <row r="188" spans="1:21" s="50" customFormat="1">
+    <row r="188" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A188" s="36"/>
       <c r="B188" s="36"/>
       <c r="C188" s="36"/>
@@ -8359,7 +8364,7 @@
       <c r="T188" s="49"/>
       <c r="U188" s="49"/>
     </row>
-    <row r="189" spans="1:21" s="50" customFormat="1">
+    <row r="189" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A189" s="36"/>
       <c r="B189" s="36"/>
       <c r="C189" s="36"/>
@@ -8382,7 +8387,7 @@
       <c r="T189" s="49"/>
       <c r="U189" s="49"/>
     </row>
-    <row r="190" spans="1:21" s="50" customFormat="1">
+    <row r="190" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A190" s="36"/>
       <c r="B190" s="36"/>
       <c r="C190" s="36"/>
@@ -8405,7 +8410,7 @@
       <c r="T190" s="49"/>
       <c r="U190" s="49"/>
     </row>
-    <row r="191" spans="1:21" s="50" customFormat="1">
+    <row r="191" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A191" s="36"/>
       <c r="B191" s="36"/>
       <c r="C191" s="36"/>
@@ -8428,7 +8433,7 @@
       <c r="T191" s="49"/>
       <c r="U191" s="49"/>
     </row>
-    <row r="192" spans="1:21" s="50" customFormat="1">
+    <row r="192" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A192" s="36"/>
       <c r="B192" s="36"/>
       <c r="C192" s="36"/>
@@ -8451,7 +8456,7 @@
       <c r="T192" s="49"/>
       <c r="U192" s="49"/>
     </row>
-    <row r="193" spans="1:21" s="50" customFormat="1">
+    <row r="193" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A193" s="36"/>
       <c r="B193" s="36"/>
       <c r="C193" s="36"/>
@@ -8474,7 +8479,7 @@
       <c r="T193" s="49"/>
       <c r="U193" s="49"/>
     </row>
-    <row r="194" spans="1:21" s="50" customFormat="1">
+    <row r="194" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A194" s="36"/>
       <c r="B194" s="36"/>
       <c r="C194" s="36"/>
@@ -8497,7 +8502,7 @@
       <c r="T194" s="49"/>
       <c r="U194" s="49"/>
     </row>
-    <row r="195" spans="1:21" s="50" customFormat="1">
+    <row r="195" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A195" s="36"/>
       <c r="B195" s="36"/>
       <c r="C195" s="36"/>
@@ -8520,7 +8525,7 @@
       <c r="T195" s="49"/>
       <c r="U195" s="49"/>
     </row>
-    <row r="196" spans="1:21" s="50" customFormat="1">
+    <row r="196" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A196" s="36"/>
       <c r="B196" s="36"/>
       <c r="C196" s="36"/>
@@ -8543,7 +8548,7 @@
       <c r="T196" s="49"/>
       <c r="U196" s="49"/>
     </row>
-    <row r="197" spans="1:21" s="50" customFormat="1">
+    <row r="197" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A197" s="36"/>
       <c r="B197" s="36"/>
       <c r="C197" s="36"/>
@@ -8566,7 +8571,7 @@
       <c r="T197" s="49"/>
       <c r="U197" s="49"/>
     </row>
-    <row r="198" spans="1:21" s="50" customFormat="1">
+    <row r="198" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A198" s="36"/>
       <c r="B198" s="36"/>
       <c r="C198" s="36"/>
@@ -8589,7 +8594,7 @@
       <c r="T198" s="49"/>
       <c r="U198" s="49"/>
     </row>
-    <row r="199" spans="1:21" s="50" customFormat="1">
+    <row r="199" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A199" s="36"/>
       <c r="B199" s="36"/>
       <c r="C199" s="36"/>
@@ -8612,7 +8617,7 @@
       <c r="T199" s="49"/>
       <c r="U199" s="49"/>
     </row>
-    <row r="200" spans="1:21" s="50" customFormat="1">
+    <row r="200" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A200" s="36"/>
       <c r="B200" s="36"/>
       <c r="C200" s="36"/>
@@ -8635,7 +8640,7 @@
       <c r="T200" s="49"/>
       <c r="U200" s="49"/>
     </row>
-    <row r="201" spans="1:21" s="50" customFormat="1">
+    <row r="201" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A201" s="36"/>
       <c r="B201" s="36"/>
       <c r="C201" s="36"/>
@@ -8658,7 +8663,7 @@
       <c r="T201" s="49"/>
       <c r="U201" s="49"/>
     </row>
-    <row r="202" spans="1:21" s="50" customFormat="1">
+    <row r="202" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A202" s="36"/>
       <c r="B202" s="36"/>
       <c r="C202" s="36"/>
@@ -8681,7 +8686,7 @@
       <c r="T202" s="49"/>
       <c r="U202" s="49"/>
     </row>
-    <row r="203" spans="1:21" s="50" customFormat="1">
+    <row r="203" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A203" s="36"/>
       <c r="B203" s="36"/>
       <c r="C203" s="36"/>
@@ -8704,7 +8709,7 @@
       <c r="T203" s="49"/>
       <c r="U203" s="49"/>
     </row>
-    <row r="204" spans="1:21" s="50" customFormat="1">
+    <row r="204" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A204" s="36"/>
       <c r="B204" s="36"/>
       <c r="C204" s="36"/>
@@ -8727,7 +8732,7 @@
       <c r="T204" s="49"/>
       <c r="U204" s="49"/>
     </row>
-    <row r="205" spans="1:21" s="50" customFormat="1">
+    <row r="205" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A205" s="36"/>
       <c r="B205" s="36"/>
       <c r="C205" s="36"/>
@@ -8750,7 +8755,7 @@
       <c r="T205" s="49"/>
       <c r="U205" s="49"/>
     </row>
-    <row r="206" spans="1:21" s="50" customFormat="1">
+    <row r="206" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A206" s="36"/>
       <c r="B206" s="36"/>
       <c r="C206" s="36"/>
@@ -8773,7 +8778,7 @@
       <c r="T206" s="49"/>
       <c r="U206" s="49"/>
     </row>
-    <row r="207" spans="1:21" s="50" customFormat="1">
+    <row r="207" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A207" s="36"/>
       <c r="B207" s="36"/>
       <c r="C207" s="36"/>
@@ -8796,7 +8801,7 @@
       <c r="T207" s="49"/>
       <c r="U207" s="49"/>
     </row>
-    <row r="208" spans="1:21" s="50" customFormat="1">
+    <row r="208" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A208" s="36"/>
       <c r="B208" s="36"/>
       <c r="C208" s="36"/>
@@ -8819,7 +8824,7 @@
       <c r="T208" s="49"/>
       <c r="U208" s="49"/>
     </row>
-    <row r="209" spans="1:21" s="50" customFormat="1">
+    <row r="209" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A209" s="36"/>
       <c r="B209" s="36"/>
       <c r="C209" s="36"/>
@@ -8842,7 +8847,7 @@
       <c r="T209" s="49"/>
       <c r="U209" s="49"/>
     </row>
-    <row r="210" spans="1:21" s="50" customFormat="1">
+    <row r="210" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A210" s="36"/>
       <c r="B210" s="36"/>
       <c r="C210" s="36"/>
@@ -8865,7 +8870,7 @@
       <c r="T210" s="49"/>
       <c r="U210" s="49"/>
     </row>
-    <row r="211" spans="1:21" s="50" customFormat="1">
+    <row r="211" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A211" s="36"/>
       <c r="B211" s="36"/>
       <c r="C211" s="36"/>
@@ -8888,7 +8893,7 @@
       <c r="T211" s="49"/>
       <c r="U211" s="49"/>
     </row>
-    <row r="212" spans="1:21" s="50" customFormat="1">
+    <row r="212" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A212" s="36"/>
       <c r="B212" s="36"/>
       <c r="C212" s="36"/>
@@ -8911,7 +8916,7 @@
       <c r="T212" s="49"/>
       <c r="U212" s="49"/>
     </row>
-    <row r="213" spans="1:21" s="50" customFormat="1">
+    <row r="213" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A213" s="36"/>
       <c r="B213" s="36"/>
       <c r="C213" s="36"/>
@@ -8934,7 +8939,7 @@
       <c r="T213" s="49"/>
       <c r="U213" s="49"/>
     </row>
-    <row r="214" spans="1:21" s="50" customFormat="1">
+    <row r="214" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A214" s="36"/>
       <c r="B214" s="36"/>
       <c r="C214" s="36"/>
@@ -8957,7 +8962,7 @@
       <c r="T214" s="49"/>
       <c r="U214" s="49"/>
     </row>
-    <row r="215" spans="1:21" s="50" customFormat="1">
+    <row r="215" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A215" s="36"/>
       <c r="B215" s="36"/>
       <c r="C215" s="36"/>
@@ -8980,7 +8985,7 @@
       <c r="T215" s="49"/>
       <c r="U215" s="49"/>
     </row>
-    <row r="216" spans="1:21" s="50" customFormat="1">
+    <row r="216" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A216" s="36"/>
       <c r="B216" s="36"/>
       <c r="C216" s="36"/>
@@ -9003,7 +9008,7 @@
       <c r="T216" s="49"/>
       <c r="U216" s="49"/>
     </row>
-    <row r="217" spans="1:21" s="50" customFormat="1">
+    <row r="217" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A217" s="36"/>
       <c r="B217" s="36"/>
       <c r="C217" s="36"/>
@@ -9026,7 +9031,7 @@
       <c r="T217" s="49"/>
       <c r="U217" s="49"/>
     </row>
-    <row r="218" spans="1:21" s="50" customFormat="1">
+    <row r="218" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A218" s="36"/>
       <c r="B218" s="36"/>
       <c r="C218" s="36"/>
@@ -9049,7 +9054,7 @@
       <c r="T218" s="49"/>
       <c r="U218" s="49"/>
     </row>
-    <row r="219" spans="1:21" s="50" customFormat="1">
+    <row r="219" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A219" s="36"/>
       <c r="B219" s="36"/>
       <c r="C219" s="36"/>
@@ -9072,7 +9077,7 @@
       <c r="T219" s="49"/>
       <c r="U219" s="49"/>
     </row>
-    <row r="220" spans="1:21" s="50" customFormat="1">
+    <row r="220" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A220" s="36"/>
       <c r="B220" s="36"/>
       <c r="C220" s="36"/>
@@ -9095,7 +9100,7 @@
       <c r="T220" s="49"/>
       <c r="U220" s="49"/>
     </row>
-    <row r="221" spans="1:21" s="50" customFormat="1">
+    <row r="221" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A221" s="36"/>
       <c r="B221" s="36"/>
       <c r="C221" s="36"/>
@@ -9118,7 +9123,7 @@
       <c r="T221" s="49"/>
       <c r="U221" s="49"/>
     </row>
-    <row r="222" spans="1:21" s="50" customFormat="1">
+    <row r="222" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A222" s="36"/>
       <c r="B222" s="36"/>
       <c r="C222" s="36"/>
@@ -9141,7 +9146,7 @@
       <c r="T222" s="49"/>
       <c r="U222" s="49"/>
     </row>
-    <row r="223" spans="1:21" s="50" customFormat="1">
+    <row r="223" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A223" s="36"/>
       <c r="B223" s="36"/>
       <c r="C223" s="36"/>
@@ -9164,7 +9169,7 @@
       <c r="T223" s="49"/>
       <c r="U223" s="49"/>
     </row>
-    <row r="224" spans="1:21" s="50" customFormat="1">
+    <row r="224" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A224" s="36"/>
       <c r="B224" s="36"/>
       <c r="C224" s="36"/>
@@ -9187,7 +9192,7 @@
       <c r="T224" s="49"/>
       <c r="U224" s="49"/>
     </row>
-    <row r="225" spans="1:21" s="50" customFormat="1">
+    <row r="225" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A225" s="36"/>
       <c r="B225" s="36"/>
       <c r="C225" s="36"/>
@@ -9210,7 +9215,7 @@
       <c r="T225" s="49"/>
       <c r="U225" s="49"/>
     </row>
-    <row r="226" spans="1:21" s="50" customFormat="1">
+    <row r="226" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A226" s="36"/>
       <c r="B226" s="36"/>
       <c r="C226" s="36"/>
@@ -9233,7 +9238,7 @@
       <c r="T226" s="49"/>
       <c r="U226" s="49"/>
     </row>
-    <row r="227" spans="1:21" s="50" customFormat="1">
+    <row r="227" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A227" s="36"/>
       <c r="B227" s="36"/>
       <c r="C227" s="36"/>
@@ -9256,7 +9261,7 @@
       <c r="T227" s="49"/>
       <c r="U227" s="49"/>
     </row>
-    <row r="228" spans="1:21" s="50" customFormat="1">
+    <row r="228" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A228" s="36"/>
       <c r="B228" s="36"/>
       <c r="C228" s="36"/>
@@ -9279,7 +9284,7 @@
       <c r="T228" s="49"/>
       <c r="U228" s="49"/>
     </row>
-    <row r="229" spans="1:21" s="50" customFormat="1">
+    <row r="229" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A229" s="36"/>
       <c r="B229" s="36"/>
       <c r="C229" s="36"/>
@@ -9302,7 +9307,7 @@
       <c r="T229" s="49"/>
       <c r="U229" s="49"/>
     </row>
-    <row r="230" spans="1:21" s="50" customFormat="1">
+    <row r="230" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A230" s="36"/>
       <c r="B230" s="36"/>
       <c r="C230" s="36"/>
@@ -9325,7 +9330,7 @@
       <c r="T230" s="49"/>
       <c r="U230" s="49"/>
     </row>
-    <row r="231" spans="1:21" s="50" customFormat="1">
+    <row r="231" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A231" s="36"/>
       <c r="B231" s="36"/>
       <c r="C231" s="36"/>
@@ -9348,7 +9353,7 @@
       <c r="T231" s="49"/>
       <c r="U231" s="49"/>
     </row>
-    <row r="232" spans="1:21" s="50" customFormat="1">
+    <row r="232" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A232" s="36"/>
       <c r="B232" s="36"/>
       <c r="C232" s="36"/>
@@ -9371,7 +9376,7 @@
       <c r="T232" s="49"/>
       <c r="U232" s="49"/>
     </row>
-    <row r="233" spans="1:21" s="50" customFormat="1">
+    <row r="233" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A233" s="36"/>
       <c r="B233" s="36"/>
       <c r="C233" s="36"/>
@@ -9394,7 +9399,7 @@
       <c r="T233" s="49"/>
       <c r="U233" s="49"/>
     </row>
-    <row r="234" spans="1:21" s="50" customFormat="1">
+    <row r="234" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A234" s="36"/>
       <c r="B234" s="36"/>
       <c r="C234" s="36"/>
@@ -9417,7 +9422,7 @@
       <c r="T234" s="49"/>
       <c r="U234" s="49"/>
     </row>
-    <row r="235" spans="1:21" s="50" customFormat="1">
+    <row r="235" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A235" s="36"/>
       <c r="B235" s="36"/>
       <c r="C235" s="36"/>
@@ -9440,7 +9445,7 @@
       <c r="T235" s="49"/>
       <c r="U235" s="49"/>
     </row>
-    <row r="236" spans="1:21" s="50" customFormat="1">
+    <row r="236" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A236" s="36"/>
       <c r="B236" s="36"/>
       <c r="C236" s="36"/>
@@ -9463,7 +9468,7 @@
       <c r="T236" s="49"/>
       <c r="U236" s="49"/>
     </row>
-    <row r="237" spans="1:21" s="50" customFormat="1">
+    <row r="237" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A237" s="36"/>
       <c r="B237" s="36"/>
       <c r="C237" s="36"/>
@@ -9486,7 +9491,7 @@
       <c r="T237" s="49"/>
       <c r="U237" s="49"/>
     </row>
-    <row r="238" spans="1:21" s="50" customFormat="1">
+    <row r="238" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A238" s="36"/>
       <c r="B238" s="36"/>
       <c r="C238" s="36"/>
@@ -9509,7 +9514,7 @@
       <c r="T238" s="49"/>
       <c r="U238" s="49"/>
     </row>
-    <row r="239" spans="1:21" s="50" customFormat="1">
+    <row r="239" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A239" s="36"/>
       <c r="B239" s="36"/>
       <c r="C239" s="36"/>
@@ -9532,7 +9537,7 @@
       <c r="T239" s="49"/>
       <c r="U239" s="49"/>
     </row>
-    <row r="240" spans="1:21" s="50" customFormat="1">
+    <row r="240" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A240" s="36"/>
       <c r="B240" s="36"/>
       <c r="C240" s="36"/>
@@ -9555,7 +9560,7 @@
       <c r="T240" s="49"/>
       <c r="U240" s="49"/>
     </row>
-    <row r="241" spans="1:21" s="50" customFormat="1">
+    <row r="241" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A241" s="36"/>
       <c r="B241" s="36"/>
       <c r="C241" s="36"/>
@@ -9578,7 +9583,7 @@
       <c r="T241" s="49"/>
       <c r="U241" s="49"/>
     </row>
-    <row r="242" spans="1:21" s="50" customFormat="1">
+    <row r="242" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A242" s="36"/>
       <c r="B242" s="36"/>
       <c r="C242" s="36"/>
@@ -9601,7 +9606,7 @@
       <c r="T242" s="49"/>
       <c r="U242" s="49"/>
     </row>
-    <row r="243" spans="1:21" s="50" customFormat="1">
+    <row r="243" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A243" s="36"/>
       <c r="B243" s="36"/>
       <c r="C243" s="36"/>
@@ -9624,7 +9629,7 @@
       <c r="T243" s="49"/>
       <c r="U243" s="49"/>
     </row>
-    <row r="244" spans="1:21" s="50" customFormat="1">
+    <row r="244" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A244" s="36"/>
       <c r="B244" s="36"/>
       <c r="C244" s="36"/>
@@ -9647,7 +9652,7 @@
       <c r="T244" s="49"/>
       <c r="U244" s="49"/>
     </row>
-    <row r="245" spans="1:21" s="50" customFormat="1">
+    <row r="245" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A245" s="36"/>
       <c r="B245" s="36"/>
       <c r="C245" s="36"/>
@@ -9670,7 +9675,7 @@
       <c r="T245" s="49"/>
       <c r="U245" s="49"/>
     </row>
-    <row r="246" spans="1:21" s="50" customFormat="1">
+    <row r="246" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A246" s="36"/>
       <c r="B246" s="36"/>
       <c r="C246" s="36"/>
@@ -9693,7 +9698,7 @@
       <c r="T246" s="49"/>
       <c r="U246" s="49"/>
     </row>
-    <row r="247" spans="1:21" s="50" customFormat="1">
+    <row r="247" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A247" s="36"/>
       <c r="B247" s="36"/>
       <c r="C247" s="36"/>
@@ -9716,7 +9721,7 @@
       <c r="T247" s="49"/>
       <c r="U247" s="49"/>
     </row>
-    <row r="248" spans="1:21" s="50" customFormat="1">
+    <row r="248" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A248" s="36"/>
       <c r="B248" s="36"/>
       <c r="C248" s="36"/>
@@ -9739,7 +9744,7 @@
       <c r="T248" s="49"/>
       <c r="U248" s="49"/>
     </row>
-    <row r="249" spans="1:21" s="50" customFormat="1">
+    <row r="249" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A249" s="36"/>
       <c r="B249" s="36"/>
       <c r="C249" s="36"/>
@@ -9762,7 +9767,7 @@
       <c r="T249" s="49"/>
       <c r="U249" s="49"/>
     </row>
-    <row r="250" spans="1:21" s="50" customFormat="1">
+    <row r="250" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A250" s="36"/>
       <c r="B250" s="36"/>
       <c r="C250" s="36"/>
@@ -9785,7 +9790,7 @@
       <c r="T250" s="49"/>
       <c r="U250" s="49"/>
     </row>
-    <row r="251" spans="1:21" s="50" customFormat="1">
+    <row r="251" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A251" s="36"/>
       <c r="B251" s="36"/>
       <c r="C251" s="36"/>
@@ -9808,7 +9813,7 @@
       <c r="T251" s="49"/>
       <c r="U251" s="49"/>
     </row>
-    <row r="252" spans="1:21" s="50" customFormat="1">
+    <row r="252" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A252" s="36"/>
       <c r="B252" s="36"/>
       <c r="C252" s="36"/>
@@ -9831,7 +9836,7 @@
       <c r="T252" s="49"/>
       <c r="U252" s="49"/>
     </row>
-    <row r="253" spans="1:21" s="50" customFormat="1">
+    <row r="253" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A253" s="36"/>
       <c r="B253" s="36"/>
       <c r="C253" s="36"/>
@@ -9854,7 +9859,7 @@
       <c r="T253" s="49"/>
       <c r="U253" s="49"/>
     </row>
-    <row r="254" spans="1:21" s="50" customFormat="1">
+    <row r="254" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A254" s="36"/>
       <c r="B254" s="36"/>
       <c r="C254" s="36"/>
@@ -9877,7 +9882,7 @@
       <c r="T254" s="49"/>
       <c r="U254" s="49"/>
     </row>
-    <row r="255" spans="1:21" s="50" customFormat="1">
+    <row r="255" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A255" s="36"/>
       <c r="B255" s="36"/>
       <c r="C255" s="36"/>
@@ -9900,7 +9905,7 @@
       <c r="T255" s="49"/>
       <c r="U255" s="49"/>
     </row>
-    <row r="256" spans="1:21" s="50" customFormat="1">
+    <row r="256" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A256" s="36"/>
       <c r="B256" s="36"/>
       <c r="C256" s="36"/>
@@ -9923,7 +9928,7 @@
       <c r="T256" s="49"/>
       <c r="U256" s="49"/>
     </row>
-    <row r="257" spans="1:21" s="50" customFormat="1">
+    <row r="257" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A257" s="36"/>
       <c r="B257" s="36"/>
       <c r="C257" s="36"/>
@@ -9946,7 +9951,7 @@
       <c r="T257" s="49"/>
       <c r="U257" s="49"/>
     </row>
-    <row r="258" spans="1:21" s="50" customFormat="1">
+    <row r="258" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A258" s="36"/>
       <c r="B258" s="36"/>
       <c r="C258" s="36"/>
@@ -9969,7 +9974,7 @@
       <c r="T258" s="49"/>
       <c r="U258" s="49"/>
     </row>
-    <row r="259" spans="1:21" s="50" customFormat="1">
+    <row r="259" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A259" s="36"/>
       <c r="B259" s="36"/>
       <c r="C259" s="36"/>
@@ -9992,7 +9997,7 @@
       <c r="T259" s="49"/>
       <c r="U259" s="49"/>
     </row>
-    <row r="260" spans="1:21" s="50" customFormat="1">
+    <row r="260" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A260" s="36"/>
       <c r="B260" s="36"/>
       <c r="C260" s="36"/>
@@ -10015,7 +10020,7 @@
       <c r="T260" s="49"/>
       <c r="U260" s="49"/>
     </row>
-    <row r="261" spans="1:21" s="50" customFormat="1">
+    <row r="261" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A261" s="36"/>
       <c r="B261" s="36"/>
       <c r="C261" s="36"/>
@@ -10038,7 +10043,7 @@
       <c r="T261" s="49"/>
       <c r="U261" s="49"/>
     </row>
-    <row r="262" spans="1:21" s="50" customFormat="1">
+    <row r="262" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A262" s="36"/>
       <c r="B262" s="36"/>
       <c r="C262" s="36"/>
@@ -10061,7 +10066,7 @@
       <c r="T262" s="49"/>
       <c r="U262" s="49"/>
     </row>
-    <row r="263" spans="1:21" s="50" customFormat="1">
+    <row r="263" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A263" s="36"/>
       <c r="B263" s="36"/>
       <c r="C263" s="36"/>
@@ -10084,7 +10089,7 @@
       <c r="T263" s="49"/>
       <c r="U263" s="49"/>
     </row>
-    <row r="264" spans="1:21" s="50" customFormat="1">
+    <row r="264" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A264" s="36"/>
       <c r="B264" s="36"/>
       <c r="C264" s="36"/>
@@ -10107,7 +10112,7 @@
       <c r="T264" s="49"/>
       <c r="U264" s="49"/>
     </row>
-    <row r="265" spans="1:21" s="50" customFormat="1">
+    <row r="265" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A265" s="36"/>
       <c r="B265" s="36"/>
       <c r="C265" s="36"/>
@@ -10130,7 +10135,7 @@
       <c r="T265" s="49"/>
       <c r="U265" s="49"/>
     </row>
-    <row r="266" spans="1:21" s="50" customFormat="1">
+    <row r="266" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A266" s="36"/>
       <c r="B266" s="36"/>
       <c r="C266" s="36"/>
@@ -10153,7 +10158,7 @@
       <c r="T266" s="49"/>
       <c r="U266" s="49"/>
     </row>
-    <row r="267" spans="1:21" s="50" customFormat="1">
+    <row r="267" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A267" s="36"/>
       <c r="B267" s="36"/>
       <c r="C267" s="36"/>
@@ -10176,7 +10181,7 @@
       <c r="T267" s="49"/>
       <c r="U267" s="49"/>
     </row>
-    <row r="268" spans="1:21" s="50" customFormat="1">
+    <row r="268" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A268" s="36"/>
       <c r="B268" s="36"/>
       <c r="C268" s="36"/>
@@ -10199,7 +10204,7 @@
       <c r="T268" s="49"/>
       <c r="U268" s="49"/>
     </row>
-    <row r="269" spans="1:21" s="50" customFormat="1">
+    <row r="269" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A269" s="36"/>
       <c r="B269" s="36"/>
       <c r="C269" s="36"/>
@@ -10222,7 +10227,7 @@
       <c r="T269" s="49"/>
       <c r="U269" s="49"/>
     </row>
-    <row r="270" spans="1:21" s="50" customFormat="1">
+    <row r="270" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A270" s="36"/>
       <c r="B270" s="36"/>
       <c r="C270" s="36"/>
@@ -10245,7 +10250,7 @@
       <c r="T270" s="49"/>
       <c r="U270" s="49"/>
     </row>
-    <row r="271" spans="1:21" s="50" customFormat="1">
+    <row r="271" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A271" s="36"/>
       <c r="B271" s="36"/>
       <c r="C271" s="36"/>
@@ -10268,7 +10273,7 @@
       <c r="T271" s="49"/>
       <c r="U271" s="49"/>
     </row>
-    <row r="272" spans="1:21" s="50" customFormat="1">
+    <row r="272" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A272" s="36"/>
       <c r="B272" s="36"/>
       <c r="C272" s="36"/>
@@ -10291,7 +10296,7 @@
       <c r="T272" s="49"/>
       <c r="U272" s="49"/>
     </row>
-    <row r="273" spans="1:21" s="50" customFormat="1">
+    <row r="273" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A273" s="36"/>
       <c r="B273" s="36"/>
       <c r="C273" s="36"/>
@@ -10314,7 +10319,7 @@
       <c r="T273" s="49"/>
       <c r="U273" s="49"/>
     </row>
-    <row r="274" spans="1:21" s="50" customFormat="1">
+    <row r="274" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A274" s="36"/>
       <c r="B274" s="36"/>
       <c r="C274" s="36"/>
@@ -10337,7 +10342,7 @@
       <c r="T274" s="49"/>
       <c r="U274" s="49"/>
     </row>
-    <row r="275" spans="1:21" s="50" customFormat="1">
+    <row r="275" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A275" s="36"/>
       <c r="B275" s="36"/>
       <c r="C275" s="36"/>
@@ -10360,7 +10365,7 @@
       <c r="T275" s="49"/>
       <c r="U275" s="49"/>
     </row>
-    <row r="276" spans="1:21" s="50" customFormat="1">
+    <row r="276" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A276" s="36"/>
       <c r="B276" s="36"/>
       <c r="C276" s="36"/>
@@ -10383,7 +10388,7 @@
       <c r="T276" s="49"/>
       <c r="U276" s="49"/>
     </row>
-    <row r="277" spans="1:21" s="50" customFormat="1">
+    <row r="277" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A277" s="36"/>
       <c r="B277" s="36"/>
       <c r="C277" s="36"/>
@@ -10406,7 +10411,7 @@
       <c r="T277" s="49"/>
       <c r="U277" s="49"/>
     </row>
-    <row r="278" spans="1:21" s="50" customFormat="1">
+    <row r="278" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A278" s="36"/>
       <c r="B278" s="36"/>
       <c r="C278" s="36"/>
@@ -10429,7 +10434,7 @@
       <c r="T278" s="49"/>
       <c r="U278" s="49"/>
     </row>
-    <row r="279" spans="1:21" s="50" customFormat="1">
+    <row r="279" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A279" s="36"/>
       <c r="B279" s="36"/>
       <c r="C279" s="36"/>
@@ -10452,7 +10457,7 @@
       <c r="T279" s="49"/>
       <c r="U279" s="49"/>
     </row>
-    <row r="280" spans="1:21" s="50" customFormat="1">
+    <row r="280" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A280" s="36"/>
       <c r="B280" s="36"/>
       <c r="C280" s="36"/>
@@ -10475,7 +10480,7 @@
       <c r="T280" s="49"/>
       <c r="U280" s="49"/>
     </row>
-    <row r="281" spans="1:21" s="50" customFormat="1">
+    <row r="281" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A281" s="36"/>
       <c r="B281" s="36"/>
       <c r="C281" s="36"/>
@@ -10498,7 +10503,7 @@
       <c r="T281" s="49"/>
       <c r="U281" s="49"/>
     </row>
-    <row r="282" spans="1:21" s="50" customFormat="1">
+    <row r="282" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A282" s="36"/>
       <c r="B282" s="36"/>
       <c r="C282" s="36"/>
@@ -10521,7 +10526,7 @@
       <c r="T282" s="49"/>
       <c r="U282" s="49"/>
     </row>
-    <row r="283" spans="1:21" s="50" customFormat="1">
+    <row r="283" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A283" s="36"/>
       <c r="B283" s="36"/>
       <c r="C283" s="36"/>
@@ -10544,7 +10549,7 @@
       <c r="T283" s="49"/>
       <c r="U283" s="49"/>
     </row>
-    <row r="284" spans="1:21" s="50" customFormat="1">
+    <row r="284" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A284" s="36"/>
       <c r="B284" s="36"/>
       <c r="C284" s="36"/>
@@ -10567,7 +10572,7 @@
       <c r="T284" s="49"/>
       <c r="U284" s="49"/>
     </row>
-    <row r="285" spans="1:21" s="50" customFormat="1">
+    <row r="285" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A285" s="36"/>
       <c r="B285" s="36"/>
       <c r="C285" s="36"/>
@@ -10590,7 +10595,7 @@
       <c r="T285" s="49"/>
       <c r="U285" s="49"/>
     </row>
-    <row r="286" spans="1:21" s="50" customFormat="1">
+    <row r="286" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A286" s="36"/>
       <c r="B286" s="36"/>
       <c r="C286" s="36"/>
@@ -10613,7 +10618,7 @@
       <c r="T286" s="49"/>
       <c r="U286" s="49"/>
     </row>
-    <row r="287" spans="1:21" s="50" customFormat="1">
+    <row r="287" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A287" s="36"/>
       <c r="B287" s="36"/>
       <c r="C287" s="36"/>
@@ -10636,7 +10641,7 @@
       <c r="T287" s="49"/>
       <c r="U287" s="49"/>
     </row>
-    <row r="288" spans="1:21" s="50" customFormat="1">
+    <row r="288" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A288" s="36"/>
       <c r="B288" s="36"/>
       <c r="C288" s="36"/>
@@ -10659,7 +10664,7 @@
       <c r="T288" s="49"/>
       <c r="U288" s="49"/>
     </row>
-    <row r="289" spans="1:21" s="50" customFormat="1">
+    <row r="289" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A289" s="36"/>
       <c r="B289" s="36"/>
       <c r="C289" s="36"/>
@@ -10682,7 +10687,7 @@
       <c r="T289" s="49"/>
       <c r="U289" s="49"/>
     </row>
-    <row r="290" spans="1:21" s="50" customFormat="1">
+    <row r="290" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A290" s="36"/>
       <c r="B290" s="36"/>
       <c r="C290" s="36"/>
@@ -10705,7 +10710,7 @@
       <c r="T290" s="49"/>
       <c r="U290" s="49"/>
     </row>
-    <row r="291" spans="1:21" s="50" customFormat="1">
+    <row r="291" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A291" s="36"/>
       <c r="B291" s="36"/>
       <c r="C291" s="36"/>
@@ -10728,7 +10733,7 @@
       <c r="T291" s="49"/>
       <c r="U291" s="49"/>
     </row>
-    <row r="292" spans="1:21" s="50" customFormat="1">
+    <row r="292" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A292" s="36"/>
       <c r="B292" s="36"/>
       <c r="C292" s="36"/>
@@ -10751,7 +10756,7 @@
       <c r="T292" s="49"/>
       <c r="U292" s="49"/>
     </row>
-    <row r="293" spans="1:21" s="50" customFormat="1">
+    <row r="293" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A293" s="36"/>
       <c r="B293" s="36"/>
       <c r="C293" s="36"/>
@@ -10774,7 +10779,7 @@
       <c r="T293" s="49"/>
       <c r="U293" s="49"/>
     </row>
-    <row r="294" spans="1:21" s="50" customFormat="1">
+    <row r="294" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A294" s="36"/>
       <c r="B294" s="36"/>
       <c r="C294" s="36"/>
@@ -10797,7 +10802,7 @@
       <c r="T294" s="49"/>
       <c r="U294" s="49"/>
     </row>
-    <row r="295" spans="1:21" s="50" customFormat="1">
+    <row r="295" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A295" s="36"/>
       <c r="B295" s="36"/>
       <c r="C295" s="36"/>
@@ -10820,7 +10825,7 @@
       <c r="T295" s="49"/>
       <c r="U295" s="49"/>
     </row>
-    <row r="296" spans="1:21" s="50" customFormat="1">
+    <row r="296" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A296" s="36"/>
       <c r="B296" s="36"/>
       <c r="C296" s="36"/>
@@ -10843,7 +10848,7 @@
       <c r="T296" s="49"/>
       <c r="U296" s="49"/>
     </row>
-    <row r="297" spans="1:21" s="50" customFormat="1">
+    <row r="297" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A297" s="36"/>
       <c r="B297" s="36"/>
       <c r="C297" s="36"/>
@@ -10866,7 +10871,7 @@
       <c r="T297" s="49"/>
       <c r="U297" s="49"/>
     </row>
-    <row r="298" spans="1:21" s="50" customFormat="1">
+    <row r="298" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A298" s="36"/>
       <c r="B298" s="36"/>
       <c r="C298" s="36"/>
@@ -10889,7 +10894,7 @@
       <c r="T298" s="49"/>
       <c r="U298" s="49"/>
     </row>
-    <row r="299" spans="1:21" s="50" customFormat="1">
+    <row r="299" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A299" s="36"/>
       <c r="B299" s="36"/>
       <c r="C299" s="36"/>
@@ -10912,7 +10917,7 @@
       <c r="T299" s="49"/>
       <c r="U299" s="49"/>
     </row>
-    <row r="300" spans="1:21" s="50" customFormat="1">
+    <row r="300" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A300" s="36"/>
       <c r="B300" s="36"/>
       <c r="C300" s="36"/>
@@ -10935,7 +10940,7 @@
       <c r="T300" s="49"/>
       <c r="U300" s="49"/>
     </row>
-    <row r="301" spans="1:21" s="50" customFormat="1">
+    <row r="301" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A301" s="36"/>
       <c r="B301" s="36"/>
       <c r="C301" s="36"/>
@@ -10958,7 +10963,7 @@
       <c r="T301" s="49"/>
       <c r="U301" s="49"/>
     </row>
-    <row r="302" spans="1:21" s="50" customFormat="1">
+    <row r="302" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A302" s="36"/>
       <c r="B302" s="36"/>
       <c r="C302" s="36"/>
@@ -10981,7 +10986,7 @@
       <c r="T302" s="49"/>
       <c r="U302" s="49"/>
     </row>
-    <row r="303" spans="1:21" s="50" customFormat="1">
+    <row r="303" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A303" s="36"/>
       <c r="B303" s="36"/>
       <c r="C303" s="36"/>
@@ -11004,7 +11009,7 @@
       <c r="T303" s="49"/>
       <c r="U303" s="49"/>
     </row>
-    <row r="304" spans="1:21" s="50" customFormat="1">
+    <row r="304" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A304" s="36"/>
       <c r="B304" s="36"/>
       <c r="C304" s="36"/>
@@ -11027,7 +11032,7 @@
       <c r="T304" s="49"/>
       <c r="U304" s="49"/>
     </row>
-    <row r="305" spans="1:21" s="50" customFormat="1">
+    <row r="305" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A305" s="36"/>
       <c r="B305" s="36"/>
       <c r="C305" s="36"/>
@@ -11050,7 +11055,7 @@
       <c r="T305" s="49"/>
       <c r="U305" s="49"/>
     </row>
-    <row r="306" spans="1:21" s="50" customFormat="1">
+    <row r="306" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A306" s="36"/>
       <c r="B306" s="36"/>
       <c r="C306" s="36"/>
@@ -11073,7 +11078,7 @@
       <c r="T306" s="49"/>
       <c r="U306" s="49"/>
     </row>
-    <row r="307" spans="1:21" s="50" customFormat="1">
+    <row r="307" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A307" s="36"/>
       <c r="B307" s="36"/>
       <c r="C307" s="36"/>
@@ -11096,7 +11101,7 @@
       <c r="T307" s="49"/>
       <c r="U307" s="49"/>
     </row>
-    <row r="308" spans="1:21" s="50" customFormat="1">
+    <row r="308" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A308" s="36"/>
       <c r="B308" s="36"/>
       <c r="C308" s="36"/>
@@ -11119,7 +11124,7 @@
       <c r="T308" s="49"/>
       <c r="U308" s="49"/>
     </row>
-    <row r="309" spans="1:21" s="50" customFormat="1">
+    <row r="309" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A309" s="36"/>
       <c r="B309" s="36"/>
       <c r="C309" s="36"/>
@@ -11142,7 +11147,7 @@
       <c r="T309" s="49"/>
       <c r="U309" s="49"/>
     </row>
-    <row r="310" spans="1:21" s="50" customFormat="1">
+    <row r="310" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A310" s="36"/>
       <c r="B310" s="36"/>
       <c r="C310" s="36"/>
@@ -11165,7 +11170,7 @@
       <c r="T310" s="49"/>
       <c r="U310" s="49"/>
     </row>
-    <row r="311" spans="1:21" s="50" customFormat="1">
+    <row r="311" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A311" s="36"/>
       <c r="B311" s="36"/>
       <c r="C311" s="36"/>
@@ -11188,7 +11193,7 @@
       <c r="T311" s="49"/>
       <c r="U311" s="49"/>
     </row>
-    <row r="312" spans="1:21" s="50" customFormat="1">
+    <row r="312" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A312" s="36"/>
       <c r="B312" s="36"/>
       <c r="C312" s="36"/>
@@ -11211,7 +11216,7 @@
       <c r="T312" s="49"/>
       <c r="U312" s="49"/>
     </row>
-    <row r="313" spans="1:21" s="50" customFormat="1">
+    <row r="313" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A313" s="36"/>
       <c r="B313" s="36"/>
       <c r="C313" s="36"/>
@@ -11234,7 +11239,7 @@
       <c r="T313" s="49"/>
       <c r="U313" s="49"/>
     </row>
-    <row r="314" spans="1:21" s="50" customFormat="1">
+    <row r="314" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A314" s="36"/>
       <c r="B314" s="36"/>
       <c r="C314" s="36"/>
@@ -11257,7 +11262,7 @@
       <c r="T314" s="49"/>
       <c r="U314" s="49"/>
     </row>
-    <row r="315" spans="1:21" s="50" customFormat="1">
+    <row r="315" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A315" s="36"/>
       <c r="B315" s="36"/>
       <c r="C315" s="36"/>
@@ -11280,7 +11285,7 @@
       <c r="T315" s="49"/>
       <c r="U315" s="49"/>
     </row>
-    <row r="316" spans="1:21" s="50" customFormat="1">
+    <row r="316" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A316" s="36"/>
       <c r="B316" s="36"/>
       <c r="C316" s="36"/>
@@ -11303,7 +11308,7 @@
       <c r="T316" s="49"/>
       <c r="U316" s="49"/>
     </row>
-    <row r="317" spans="1:21" s="50" customFormat="1">
+    <row r="317" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A317" s="36"/>
       <c r="B317" s="36"/>
       <c r="C317" s="36"/>
@@ -11326,7 +11331,7 @@
       <c r="T317" s="49"/>
       <c r="U317" s="49"/>
     </row>
-    <row r="318" spans="1:21" s="50" customFormat="1">
+    <row r="318" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A318" s="36"/>
       <c r="B318" s="36"/>
       <c r="C318" s="36"/>
@@ -11349,7 +11354,7 @@
       <c r="T318" s="49"/>
       <c r="U318" s="49"/>
     </row>
-    <row r="319" spans="1:21" s="50" customFormat="1">
+    <row r="319" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A319" s="36"/>
       <c r="B319" s="36"/>
       <c r="C319" s="36"/>
@@ -11372,7 +11377,7 @@
       <c r="T319" s="49"/>
       <c r="U319" s="49"/>
     </row>
-    <row r="320" spans="1:21" s="50" customFormat="1">
+    <row r="320" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A320" s="36"/>
       <c r="B320" s="36"/>
       <c r="C320" s="36"/>
@@ -11395,7 +11400,7 @@
       <c r="T320" s="49"/>
       <c r="U320" s="49"/>
     </row>
-    <row r="321" spans="1:21" s="50" customFormat="1">
+    <row r="321" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A321" s="36"/>
       <c r="B321" s="36"/>
       <c r="C321" s="36"/>
@@ -11418,7 +11423,7 @@
       <c r="T321" s="49"/>
       <c r="U321" s="49"/>
     </row>
-    <row r="322" spans="1:21" s="50" customFormat="1">
+    <row r="322" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A322" s="36"/>
       <c r="B322" s="36"/>
       <c r="C322" s="36"/>
@@ -11441,7 +11446,7 @@
       <c r="T322" s="49"/>
       <c r="U322" s="49"/>
     </row>
-    <row r="323" spans="1:21" s="50" customFormat="1">
+    <row r="323" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A323" s="36"/>
       <c r="B323" s="36"/>
       <c r="C323" s="36"/>
@@ -11464,7 +11469,7 @@
       <c r="T323" s="49"/>
       <c r="U323" s="49"/>
     </row>
-    <row r="324" spans="1:21" s="50" customFormat="1">
+    <row r="324" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A324" s="36"/>
       <c r="B324" s="36"/>
       <c r="C324" s="36"/>
@@ -11487,7 +11492,7 @@
       <c r="T324" s="49"/>
       <c r="U324" s="49"/>
     </row>
-    <row r="325" spans="1:21" s="50" customFormat="1">
+    <row r="325" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A325" s="36"/>
       <c r="B325" s="36"/>
       <c r="C325" s="36"/>
@@ -11510,7 +11515,7 @@
       <c r="T325" s="49"/>
       <c r="U325" s="49"/>
     </row>
-    <row r="326" spans="1:21" s="50" customFormat="1">
+    <row r="326" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A326" s="36"/>
       <c r="B326" s="36"/>
       <c r="C326" s="36"/>
@@ -11533,7 +11538,7 @@
       <c r="T326" s="49"/>
       <c r="U326" s="49"/>
     </row>
-    <row r="327" spans="1:21" s="50" customFormat="1">
+    <row r="327" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A327" s="36"/>
       <c r="B327" s="36"/>
       <c r="C327" s="36"/>
@@ -11556,7 +11561,7 @@
       <c r="T327" s="49"/>
       <c r="U327" s="49"/>
     </row>
-    <row r="328" spans="1:21" s="50" customFormat="1">
+    <row r="328" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A328" s="36"/>
       <c r="B328" s="36"/>
       <c r="C328" s="36"/>
@@ -11579,7 +11584,7 @@
       <c r="T328" s="49"/>
       <c r="U328" s="49"/>
     </row>
-    <row r="329" spans="1:21" s="50" customFormat="1">
+    <row r="329" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A329" s="33"/>
       <c r="B329" s="33"/>
       <c r="C329" s="33"/>
@@ -11602,7 +11607,7 @@
       <c r="T329" s="65"/>
       <c r="U329" s="65"/>
     </row>
-    <row r="330" spans="1:21" s="50" customFormat="1">
+    <row r="330" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A330" s="30"/>
       <c r="B330" s="30"/>
       <c r="C330" s="30"/>
@@ -11619,7 +11624,7 @@
       <c r="P330" s="32"/>
       <c r="Q330" s="32"/>
     </row>
-    <row r="331" spans="1:21" s="50" customFormat="1">
+    <row r="331" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A331" s="30"/>
       <c r="B331" s="30"/>
       <c r="C331" s="30"/>
@@ -11636,7 +11641,7 @@
       <c r="P331" s="32"/>
       <c r="Q331" s="32"/>
     </row>
-    <row r="332" spans="1:21" s="50" customFormat="1">
+    <row r="332" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A332" s="30"/>
       <c r="B332" s="30"/>
       <c r="C332" s="30"/>
@@ -11653,7 +11658,7 @@
       <c r="P332" s="32"/>
       <c r="Q332" s="32"/>
     </row>
-    <row r="333" spans="1:21" s="50" customFormat="1">
+    <row r="333" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A333" s="30"/>
       <c r="B333" s="30"/>
       <c r="C333" s="30"/>
@@ -11670,7 +11675,7 @@
       <c r="P333" s="32"/>
       <c r="Q333" s="32"/>
     </row>
-    <row r="334" spans="1:21" s="50" customFormat="1">
+    <row r="334" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A334" s="30"/>
       <c r="B334" s="30"/>
       <c r="C334" s="30"/>
@@ -11692,14 +11697,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="U1:U2"/>
@@ -11712,6 +11709,14 @@
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -11771,16 +11776,16 @@
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.46484375" customWidth="1"/>
+    <col min="4" max="4" width="13.796875" customWidth="1"/>
+    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.46484375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
@@ -11803,7 +11808,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>34</v>
@@ -11824,7 +11829,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>35</v>
@@ -11845,7 +11850,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>36</v>
@@ -11862,7 +11867,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>37</v>
@@ -11879,7 +11884,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>38</v>
@@ -11894,7 +11899,7 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>39</v>
@@ -11907,7 +11912,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>40</v>
@@ -11920,7 +11925,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>41</v>
@@ -11933,7 +11938,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>42</v>
@@ -11946,7 +11951,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>43</v>
@@ -11961,7 +11966,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
         <v>44</v>
@@ -11976,7 +11981,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>45</v>
@@ -11991,7 +11996,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>46</v>
@@ -12006,7 +12011,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
@@ -12019,7 +12024,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
@@ -12032,7 +12037,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
@@ -12045,7 +12050,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
@@ -12058,7 +12063,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
@@ -12071,7 +12076,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
@@ -12084,7 +12089,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
@@ -12097,7 +12102,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
@@ -12110,7 +12115,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
@@ -12123,7 +12128,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
@@ -12136,7 +12141,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
@@ -12147,7 +12152,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
@@ -12158,7 +12163,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
@@ -12169,7 +12174,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
@@ -12180,7 +12185,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
@@ -12191,7 +12196,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
@@ -12202,7 +12207,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
@@ -12213,7 +12218,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
@@ -12224,7 +12229,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
@@ -12235,7 +12240,7 @@
       <c r="F33" s="4"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
@@ -12246,7 +12251,7 @@
       <c r="F34" s="4"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
@@ -12257,7 +12262,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
@@ -12268,7 +12273,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="4" t="s">
@@ -12279,7 +12284,7 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
@@ -12290,7 +12295,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
@@ -12301,7 +12306,7 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -12310,7 +12315,7 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -12319,7 +12324,7 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -12328,7 +12333,7 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -12337,7 +12342,7 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -12346,7 +12351,7 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -12355,7 +12360,7 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -12364,7 +12369,7 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -12373,7 +12378,7 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -12382,7 +12387,7 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -12391,7 +12396,7 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>

</xml_diff>

<commit_message>
Subido cuaderno de estudio LE_07_01_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/Escaleta_LE_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/Escaleta_LE_07_01_CO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14490"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1111,11 +1111,11 @@
     <t xml:space="preserve"> Refuerza tu aprendizaje: Analiza los fragmentos de un diario</t>
   </si>
   <si>
-    <t>Actividad para leer textos líricos (poemas) en los que reconoce afinidades y distancias con su propia experiencia y efectos posibles a
+    <t>Refuerza tu aprendizaje: Rellena los espacios  con la grafía correcta</t>
+  </si>
+  <si>
+    <t>Actividad para leer textos líricos (poemas) en los que reconoce efectos posibles a
 partir del uso particular del lenguaje</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: Rellena los espacios  con la grafía correcta</t>
   </si>
 </sst>
 </file>
@@ -1568,20 +1568,20 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -1886,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="F43" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1918,94 +1918,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="92" t="s">
+      <c r="F1" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="92" t="s">
+      <c r="G1" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="92" t="s">
+      <c r="H1" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="92" t="s">
+      <c r="I1" s="95" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="92" t="s">
+      <c r="K1" s="95" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="92" t="s">
+      <c r="L1" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="92" t="s">
+      <c r="M1" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92" t="s">
+      <c r="N1" s="95"/>
+      <c r="O1" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="92" t="s">
+      <c r="P1" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="92" t="s">
+      <c r="Q1" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="92" t="s">
+      <c r="R1" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="92" t="s">
+      <c r="S1" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="92" t="s">
+      <c r="T1" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="92" t="s">
+      <c r="U1" s="95" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:52" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
+      <c r="A2" s="95"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
       <c r="J2" s="94"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
       <c r="M2" s="47" t="s">
         <v>86</v>
       </c>
       <c r="N2" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
-      <c r="Q2" s="92"/>
-      <c r="R2" s="92"/>
-      <c r="S2" s="92"/>
-      <c r="T2" s="92"/>
-      <c r="U2" s="92"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
+      <c r="Q2" s="95"/>
+      <c r="R2" s="95"/>
+      <c r="S2" s="95"/>
+      <c r="T2" s="95"/>
+      <c r="U2" s="95"/>
       <c r="V2" s="52"/>
       <c r="W2" s="52"/>
       <c r="X2" s="52"/>
@@ -4202,7 +4202,7 @@
       </c>
       <c r="F39" s="13"/>
       <c r="G39" s="24" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H39" s="13">
         <v>37</v>
@@ -4790,7 +4790,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="49" spans="1:52" s="63" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:52" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="41" t="s">
         <v>68</v>
       </c>
@@ -4808,14 +4808,14 @@
       <c r="G49" s="88" t="s">
         <v>128</v>
       </c>
-      <c r="H49" s="95">
+      <c r="H49" s="92">
         <v>47</v>
       </c>
-      <c r="I49" s="95" t="s">
+      <c r="I49" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="J49" s="96" t="s">
-        <v>310</v>
+      <c r="J49" s="93" t="s">
+        <v>311</v>
       </c>
       <c r="K49" s="13" t="s">
         <v>70</v>
@@ -11727,6 +11727,14 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="U1:U2"/>
@@ -11739,14 +11747,6 @@
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>